<commit_message>
changed typos in spreadsheet; clarified agent documentation
</commit_message>
<xml_diff>
--- a/templates/extended_aspace_import_excel_template.xlsx
+++ b/templates/extended_aspace_import_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbi\Documents\aspace\archivesspace\plugins\aspace-import-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A678D0-4197-439F-8D83-123A18B4B1E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8FC37A-E4CA-4E49-8CF4-7C4FF104EB05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="309">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -600,9 +600,6 @@
     <t>Family Agent header string</t>
   </si>
   <si>
-    <t>Corporate Agent header string</t>
-  </si>
-  <si>
     <t>Subject Source
 (If the subject term is created through this ingest, the source will  default to "Unspecified ingested source" unless the supplied Source value exactly matches an existing  controlled Source term.)</t>
   </si>
@@ -950,6 +947,15 @@
   </si>
   <si>
     <t xml:space="preserve">Person Agent Relator </t>
+  </si>
+  <si>
+    <t>Corporate Agent Record (1) ID</t>
+  </si>
+  <si>
+    <t>Corporate Agent(1) header string</t>
+  </si>
+  <si>
+    <t>Corporate Agent(1) Role</t>
   </si>
 </sst>
 </file>
@@ -1840,9 +1846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AOY7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM3" sqref="AM3"/>
+      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1:AS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,8 +1889,8 @@
     <col min="42" max="42" width="15.28515625" style="1" customWidth="1"/>
     <col min="43" max="43" width="9.140625" style="1"/>
     <col min="44" max="44" width="15.140625" style="1" customWidth="1"/>
-    <col min="45" max="45" width="15.28515625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="20.140625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="20.140625" style="1" customWidth="1"/>
+    <col min="46" max="46" width="15.28515625" style="1" customWidth="1"/>
     <col min="47" max="47" width="12.85546875" style="1" customWidth="1"/>
     <col min="48" max="48" width="9.140625" style="1"/>
     <col min="49" max="49" width="11.42578125" style="1" customWidth="1"/>
@@ -1941,7 +1947,7 @@
   <sheetData>
     <row r="1" spans="1:103" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:103" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2077,10 +2083,10 @@
       <c r="AR2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AS2" s="48" t="s">
+      <c r="AS2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AT2" s="19" t="s">
+      <c r="AT2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="AU2" s="19" t="s">
@@ -2263,7 +2269,7 @@
         <v>101</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>109</v>
@@ -2327,10 +2333,10 @@
         <v>39</v>
       </c>
       <c r="Y3" s="49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z3" s="49" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AA3" s="54" t="s">
         <v>97</v>
@@ -2366,10 +2372,10 @@
         <v>184</v>
       </c>
       <c r="AL3" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AM3" s="27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AN3" s="27" t="s">
         <v>182</v>
@@ -2378,19 +2384,19 @@
         <v>184</v>
       </c>
       <c r="AP3" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AQ3" s="27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AR3" s="27" t="s">
         <v>182</v>
       </c>
       <c r="AS3" s="27" t="s">
-        <v>275</v>
+        <v>184</v>
       </c>
       <c r="AT3" s="27" t="s">
-        <v>184</v>
+        <v>274</v>
       </c>
       <c r="AU3" s="27" t="s">
         <v>181</v>
@@ -2402,10 +2408,10 @@
         <v>185</v>
       </c>
       <c r="AX3" s="27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AY3" s="27" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AZ3" s="27" t="s">
         <v>187</v>
@@ -2414,10 +2420,10 @@
         <v>186</v>
       </c>
       <c r="BB3" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="BC3" s="27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="BD3" s="27" t="s">
         <v>187</v>
@@ -2426,7 +2432,7 @@
         <v>186</v>
       </c>
       <c r="BF3" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="BG3" s="27" t="s">
         <v>188</v>
@@ -2441,7 +2447,7 @@
         <v>126</v>
       </c>
       <c r="BK3" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BL3" s="27" t="s">
         <v>172</v>
@@ -2453,115 +2459,115 @@
         <v>126</v>
       </c>
       <c r="BO3" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BP3" s="26" t="s">
         <v>143</v>
       </c>
       <c r="BQ3" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BR3" s="26" t="s">
         <v>144</v>
       </c>
       <c r="BS3" s="59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BT3" s="26" t="s">
         <v>145</v>
       </c>
       <c r="BU3" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BV3" s="26" t="s">
         <v>146</v>
       </c>
       <c r="BW3" s="59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BX3" s="26" t="s">
         <v>147</v>
       </c>
       <c r="BY3" s="59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BZ3" s="26" t="s">
         <v>148</v>
       </c>
       <c r="CA3" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="CB3" s="26" t="s">
         <v>149</v>
       </c>
       <c r="CC3" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="CD3" s="26" t="s">
         <v>150</v>
       </c>
       <c r="CE3" s="59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="CF3" s="26" t="s">
         <v>152</v>
       </c>
       <c r="CG3" s="59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="CH3" s="26" t="s">
         <v>153</v>
       </c>
       <c r="CI3" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="CJ3" s="26" t="s">
         <v>155</v>
       </c>
       <c r="CK3" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="CL3" s="26" t="s">
         <v>156</v>
       </c>
       <c r="CM3" s="59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="CN3" s="26" t="s">
         <v>157</v>
       </c>
       <c r="CO3" s="59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="CP3" s="26" t="s">
         <v>158</v>
       </c>
       <c r="CQ3" s="59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="CR3" s="26" t="s">
         <v>159</v>
       </c>
       <c r="CS3" s="59" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CT3" s="26" t="s">
         <v>161</v>
       </c>
       <c r="CU3" s="59" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CV3" s="26" t="s">
         <v>163</v>
       </c>
       <c r="CW3" s="59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="CX3" s="26" t="s">
         <v>165</v>
       </c>
       <c r="CY3" s="59" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:103" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2590,7 +2596,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J4" s="38" t="s">
         <v>123</v>
@@ -2638,7 +2644,7 @@
         <v>40</v>
       </c>
       <c r="Y4" s="38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z4" s="38" t="s">
         <v>9</v>
@@ -2668,79 +2674,79 @@
         <v>45</v>
       </c>
       <c r="AI4" s="38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AJ4" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK4" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="AL4" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="AM4" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="AN4" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="AO4" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="AP4" s="38" t="s">
+        <v>289</v>
+      </c>
+      <c r="AQ4" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="AR4" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="AS4" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="AT4" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU4" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="AV4" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="AK4" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="AL4" s="38" t="s">
-        <v>276</v>
-      </c>
-      <c r="AM4" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="AN4" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="AO4" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="AP4" s="38" t="s">
-        <v>290</v>
-      </c>
-      <c r="AQ4" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="AR4" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="AS4" s="38" t="s">
-        <v>293</v>
-      </c>
-      <c r="AT4" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="AU4" s="38" t="s">
+      <c r="AW4" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX4" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="AY4" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ4" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="AV4" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="AW4" s="38" t="s">
-        <v>210</v>
-      </c>
-      <c r="AX4" s="38" t="s">
-        <v>297</v>
-      </c>
-      <c r="AY4" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="AZ4" s="38" t="s">
+      <c r="BA4" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="BA4" s="38" t="s">
+      <c r="BB4" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="BC4" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="BB4" s="38" t="s">
+      <c r="BD4" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="BE4" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="BF4" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="BC4" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="BD4" s="38" t="s">
+      <c r="BG4" s="38" t="s">
         <v>203</v>
-      </c>
-      <c r="BE4" s="38" t="s">
-        <v>205</v>
-      </c>
-      <c r="BF4" s="38" t="s">
-        <v>303</v>
-      </c>
-      <c r="BG4" s="38" t="s">
-        <v>204</v>
       </c>
       <c r="BH4" s="38" t="s">
         <v>173</v>
@@ -2770,109 +2776,109 @@
         <v>55</v>
       </c>
       <c r="BQ4" s="38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="BR4" s="38" t="s">
         <v>59</v>
       </c>
       <c r="BS4" s="38" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BT4" s="41" t="s">
         <v>62</v>
       </c>
       <c r="BU4" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BV4" s="38" t="s">
         <v>57</v>
       </c>
       <c r="BW4" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BX4" s="38" t="s">
         <v>58</v>
       </c>
       <c r="BY4" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BZ4" s="41" t="s">
         <v>61</v>
       </c>
       <c r="CA4" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="CB4" s="41" t="s">
         <v>118</v>
       </c>
       <c r="CC4" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="CD4" s="41" t="s">
         <v>65</v>
       </c>
       <c r="CE4" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="CF4" s="41" t="s">
         <v>63</v>
       </c>
       <c r="CG4" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="CH4" s="38" t="s">
         <v>60</v>
       </c>
       <c r="CI4" s="38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="CJ4" s="38" t="s">
         <v>119</v>
       </c>
       <c r="CK4" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="CL4" s="38" t="s">
         <v>120</v>
       </c>
       <c r="CM4" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="CN4" s="41" t="s">
         <v>91</v>
       </c>
       <c r="CO4" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="CP4" s="38" t="s">
         <v>56</v>
       </c>
       <c r="CQ4" s="38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="CR4" s="41" t="s">
         <v>67</v>
       </c>
       <c r="CS4" s="38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="CT4" s="38" t="s">
         <v>90</v>
       </c>
       <c r="CU4" s="38" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="CV4" s="41" t="s">
         <v>66</v>
       </c>
       <c r="CW4" s="41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="CX4" s="41" t="s">
         <v>64</v>
       </c>
       <c r="CY4" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:103" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2901,7 +2907,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>167</v>
@@ -2949,7 +2955,7 @@
         <v>4</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>32</v>
@@ -2982,40 +2988,40 @@
         <v>47</v>
       </c>
       <c r="AJ5" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="AN5" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="AL5" s="4" t="s">
+      <c r="AO5" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AP5" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="AM5" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="AN5" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="AP5" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="AR5" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="AS5" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="AS5" s="4" t="s">
-        <v>294</v>
-      </c>
       <c r="AT5" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="AU5" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>283</v>
       </c>
       <c r="AV5" s="4" t="s">
         <v>183</v>
@@ -3024,34 +3030,34 @@
         <v>189</v>
       </c>
       <c r="AX5" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AY5" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="BA5" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="BC5" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="AZ5" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="BA5" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="BB5" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="BC5" s="4" t="s">
-        <v>299</v>
-      </c>
       <c r="BD5" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="BE5" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="BE5" s="4" t="s">
-        <v>207</v>
-      </c>
       <c r="BF5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="BG5" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="BH5" s="4" t="s">
         <v>178</v>
@@ -3081,109 +3087,109 @@
         <v>42</v>
       </c>
       <c r="BQ5" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BR5" s="4" t="s">
         <v>49</v>
       </c>
       <c r="BS5" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BT5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="BU5" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BV5" s="4" t="s">
         <v>83</v>
       </c>
       <c r="BW5" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BX5" s="4" t="s">
         <v>48</v>
       </c>
       <c r="BY5" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BZ5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="CA5" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="CB5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="CC5" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="CD5" s="7" t="s">
         <v>84</v>
       </c>
       <c r="CE5" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CF5" s="7" t="s">
         <v>151</v>
       </c>
       <c r="CG5" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="CH5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="CI5" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="CJ5" s="4" t="s">
         <v>154</v>
       </c>
       <c r="CK5" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="CL5" s="4" t="s">
         <v>121</v>
       </c>
       <c r="CM5" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CN5" s="14" t="s">
         <v>92</v>
       </c>
       <c r="CO5" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="CP5" s="4" t="s">
         <v>69</v>
       </c>
       <c r="CQ5" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="CR5" s="7" t="s">
         <v>160</v>
       </c>
       <c r="CS5" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CT5" s="4" t="s">
         <v>162</v>
       </c>
       <c r="CU5" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CV5" s="7" t="s">
         <v>164</v>
       </c>
       <c r="CW5" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="CX5" s="7" t="s">
         <v>166</v>
       </c>
       <c r="CY5" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:103" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3218,7 +3224,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AL6:AL1048576 AP6:AP1048576 AS6:AS1048576 AX6:AX1048576 BB6:BB1048576 BF6:BF1048576</xm:sqref>
+          <xm:sqref>AL6:AL1048576 AP6:AP1048576 AX6:AX1048576 BB6:BB1048576 BF6:BF1048576 AT6:AT1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3301,17 +3307,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more agents to template, document
</commit_message>
<xml_diff>
--- a/templates/extended_aspace_import_excel_template.xlsx
+++ b/templates/extended_aspace_import_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbi\Documents\aspace\archivesspace\plugins\aspace-import-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8FC37A-E4CA-4E49-8CF4-7C4FF104EB05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA5EF00-85EB-46C3-9BA1-7941A4081E69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="342">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -569,9 +569,6 @@
     <t>Subject (1) Source</t>
   </si>
   <si>
-    <t>Creator Person Relator</t>
-  </si>
-  <si>
     <t>Person Agent Record ID
 (The numeric suffix on the URL of the Agent record, e.g., 9921 for  https://arstaffqa.hul.harvard.edu/agents/agent_person/9921</t>
   </si>
@@ -597,9 +594,6 @@
     <t>Creator CorporateRelator</t>
   </si>
   <si>
-    <t>Family Agent header string</t>
-  </si>
-  <si>
     <t>Subject Source
 (If the subject term is created through this ingest, the source will  default to "Unspecified ingested source" unless the supplied Source value exactly matches an existing  controlled Source term.)</t>
   </si>
@@ -916,9 +910,6 @@
     <t>Family Agent Role (Default: Creator)</t>
   </si>
   <si>
-    <t>Family Agent Role</t>
-  </si>
-  <si>
     <t>families_agent_role_1</t>
   </si>
   <si>
@@ -928,9 +919,6 @@
     <t>CorporateRelator(1)</t>
   </si>
   <si>
-    <t>Corporate Relator</t>
-  </si>
-  <si>
     <t>Corporate Agent Role (Default: Creator)</t>
   </si>
   <si>
@@ -949,13 +937,124 @@
     <t xml:space="preserve">Person Agent Relator </t>
   </si>
   <si>
-    <t>Corporate Agent Record (1) ID</t>
-  </si>
-  <si>
-    <t>Corporate Agent(1) header string</t>
-  </si>
-  <si>
-    <t>Corporate Agent(1) Role</t>
+    <t>Family Agent(1) Record ID</t>
+  </si>
+  <si>
+    <t>Family Agent(1) header string</t>
+  </si>
+  <si>
+    <t>Family Agent(1) Role</t>
+  </si>
+  <si>
+    <t>Family Agent(1) Relator</t>
+  </si>
+  <si>
+    <t>families_agent_record_id_2</t>
+  </si>
+  <si>
+    <t>Family Agent(2) Relator</t>
+  </si>
+  <si>
+    <t>Family Agent(2) Record ID</t>
+  </si>
+  <si>
+    <t>families_agent_header_2</t>
+  </si>
+  <si>
+    <t>Family Agent(2) header string</t>
+  </si>
+  <si>
+    <t>families_agent_role_2</t>
+  </si>
+  <si>
+    <t>Family Agent(2) Role</t>
+  </si>
+  <si>
+    <t>families_agent_relator_2</t>
+  </si>
+  <si>
+    <t>Corporate Agent Record ID(1)</t>
+  </si>
+  <si>
+    <t>Corporate Agent header string(1)</t>
+  </si>
+  <si>
+    <t>Corporate Agent Role(1)</t>
+  </si>
+  <si>
+    <t>corporate_entities_agent_record_id_3</t>
+  </si>
+  <si>
+    <t>Corporate Agent Record ID(3)</t>
+  </si>
+  <si>
+    <t>corporate_entities_agent_header_3</t>
+  </si>
+  <si>
+    <t>Corporate Agent header string(3)</t>
+  </si>
+  <si>
+    <t>corporate_entities_agent_role_3</t>
+  </si>
+  <si>
+    <t>Corporate Agent Role(3)</t>
+  </si>
+  <si>
+    <t>corporate_entities_agent_relator_3</t>
+  </si>
+  <si>
+    <t>CorporateRelator(3)</t>
+  </si>
+  <si>
+    <t>Person Agent Relator</t>
+  </si>
+  <si>
+    <t>people_agent_record_id_4</t>
+  </si>
+  <si>
+    <t>Agent(4) Record ID</t>
+  </si>
+  <si>
+    <t>people_agent_header_4</t>
+  </si>
+  <si>
+    <t>Agent(4) header string</t>
+  </si>
+  <si>
+    <t>people_agent_role_4</t>
+  </si>
+  <si>
+    <t>Agent(4) Role</t>
+  </si>
+  <si>
+    <t>people_agent_relator_4</t>
+  </si>
+  <si>
+    <t>Agent(4) Relator</t>
+  </si>
+  <si>
+    <t>people_agent_record_id_5</t>
+  </si>
+  <si>
+    <t>Agent(5) Record ID</t>
+  </si>
+  <si>
+    <t>people_agent_header_5</t>
+  </si>
+  <si>
+    <t>Agent(5) header string</t>
+  </si>
+  <si>
+    <t>people_agent_role_5</t>
+  </si>
+  <si>
+    <t>Agent(5) Role</t>
+  </si>
+  <si>
+    <t>people_agent_relator_5</t>
+  </si>
+  <si>
+    <t>Agent(5) Relator</t>
   </si>
 </sst>
 </file>
@@ -1844,11 +1943,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AOY7"/>
+  <dimension ref="A1:APO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1:AS1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,65 +1991,77 @@
     <col min="45" max="45" width="20.140625" style="1" customWidth="1"/>
     <col min="46" max="46" width="15.28515625" style="1" customWidth="1"/>
     <col min="47" max="47" width="12.85546875" style="1" customWidth="1"/>
-    <col min="48" max="48" width="9.140625" style="1"/>
-    <col min="49" max="49" width="11.42578125" style="1" customWidth="1"/>
+    <col min="48" max="48" width="15.140625" style="1" customWidth="1"/>
+    <col min="49" max="49" width="20.140625" style="1" customWidth="1"/>
     <col min="50" max="50" width="15.28515625" style="1" customWidth="1"/>
-    <col min="51" max="52" width="9.140625" style="1"/>
-    <col min="53" max="53" width="22.7109375" style="1"/>
+    <col min="51" max="51" width="12.85546875" style="1" customWidth="1"/>
+    <col min="52" max="52" width="15.140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="20.140625" style="1" customWidth="1"/>
     <col min="54" max="54" width="15.28515625" style="1" customWidth="1"/>
-    <col min="55" max="57" width="9.140625" style="1"/>
+    <col min="55" max="55" width="12.85546875" style="1" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="1"/>
+    <col min="57" max="57" width="11.42578125" style="1" customWidth="1"/>
     <col min="58" max="58" width="15.28515625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="9.140625" style="1"/>
-    <col min="60" max="60" width="11.5703125" style="1" customWidth="1"/>
-    <col min="61" max="61" width="12.28515625" style="1" customWidth="1"/>
-    <col min="62" max="64" width="13.5703125" style="1" customWidth="1"/>
-    <col min="65" max="66" width="10.85546875" style="1" customWidth="1"/>
-    <col min="67" max="67" width="15.42578125" style="1" customWidth="1"/>
-    <col min="68" max="68" width="9.28515625" style="1"/>
-    <col min="69" max="69" width="17.7109375" style="1" customWidth="1"/>
-    <col min="70" max="70" width="17" style="1" customWidth="1"/>
-    <col min="71" max="71" width="17.7109375" style="1" customWidth="1"/>
-    <col min="72" max="72" width="12.28515625" style="1" customWidth="1"/>
-    <col min="73" max="73" width="17.7109375" style="1" customWidth="1"/>
-    <col min="74" max="74" width="11.7109375" style="1" customWidth="1"/>
-    <col min="75" max="75" width="17.7109375" style="1" customWidth="1"/>
-    <col min="76" max="76" width="16" style="1" customWidth="1"/>
-    <col min="77" max="77" width="17.7109375" style="1" customWidth="1"/>
-    <col min="78" max="78" width="9.140625" style="1"/>
-    <col min="79" max="79" width="17.7109375" style="1" customWidth="1"/>
-    <col min="80" max="80" width="12" customWidth="1"/>
-    <col min="81" max="81" width="17.7109375" style="1" customWidth="1"/>
-    <col min="82" max="82" width="11.85546875" style="1" customWidth="1"/>
-    <col min="83" max="83" width="17.7109375" style="1" customWidth="1"/>
-    <col min="84" max="84" width="11.85546875" style="1" customWidth="1"/>
+    <col min="59" max="60" width="9.140625" style="1"/>
+    <col min="61" max="61" width="11.42578125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="15.28515625" style="1" customWidth="1"/>
+    <col min="63" max="65" width="9.140625" style="1"/>
+    <col min="66" max="66" width="15.28515625" style="1" customWidth="1"/>
+    <col min="67" max="69" width="9.140625" style="1"/>
+    <col min="70" max="70" width="15.28515625" style="1" customWidth="1"/>
+    <col min="71" max="73" width="9.140625" style="1"/>
+    <col min="74" max="74" width="15.28515625" style="1" customWidth="1"/>
+    <col min="75" max="75" width="9.140625" style="1"/>
+    <col min="76" max="76" width="11.5703125" style="1" customWidth="1"/>
+    <col min="77" max="77" width="12.28515625" style="1" customWidth="1"/>
+    <col min="78" max="80" width="13.5703125" style="1" customWidth="1"/>
+    <col min="81" max="82" width="10.85546875" style="1" customWidth="1"/>
+    <col min="83" max="83" width="15.42578125" style="1" customWidth="1"/>
+    <col min="84" max="84" width="9.28515625" style="1"/>
     <col min="85" max="85" width="17.7109375" style="1" customWidth="1"/>
-    <col min="86" max="86" width="11.85546875" style="1" customWidth="1"/>
+    <col min="86" max="86" width="17" style="1" customWidth="1"/>
     <col min="87" max="87" width="17.7109375" style="1" customWidth="1"/>
-    <col min="88" max="88" width="11.85546875" style="1" customWidth="1"/>
+    <col min="88" max="88" width="12.28515625" style="1" customWidth="1"/>
     <col min="89" max="89" width="17.7109375" style="1" customWidth="1"/>
-    <col min="90" max="90" width="11.85546875" style="1" customWidth="1"/>
+    <col min="90" max="90" width="11.7109375" style="1" customWidth="1"/>
     <col min="91" max="91" width="17.7109375" style="1" customWidth="1"/>
-    <col min="92" max="92" width="14.85546875" style="1" customWidth="1"/>
+    <col min="92" max="92" width="16" style="1" customWidth="1"/>
     <col min="93" max="93" width="17.7109375" style="1" customWidth="1"/>
-    <col min="94" max="94" width="12.28515625" style="1" customWidth="1"/>
+    <col min="94" max="94" width="9.140625" style="1"/>
     <col min="95" max="95" width="17.7109375" style="1" customWidth="1"/>
-    <col min="96" max="96" width="9.140625" style="1"/>
+    <col min="96" max="96" width="12" customWidth="1"/>
     <col min="97" max="97" width="17.7109375" style="1" customWidth="1"/>
-    <col min="98" max="98" width="9.140625" style="1"/>
+    <col min="98" max="98" width="11.85546875" style="1" customWidth="1"/>
     <col min="99" max="99" width="17.7109375" style="1" customWidth="1"/>
-    <col min="100" max="100" width="18.42578125" style="1" customWidth="1"/>
+    <col min="100" max="100" width="11.85546875" style="1" customWidth="1"/>
     <col min="101" max="101" width="17.7109375" style="1" customWidth="1"/>
-    <col min="102" max="102" width="10.140625" style="1" customWidth="1"/>
+    <col min="102" max="102" width="11.85546875" style="1" customWidth="1"/>
     <col min="103" max="103" width="17.7109375" style="1" customWidth="1"/>
-    <col min="104" max="1091" width="9.28515625" style="1"/>
+    <col min="104" max="104" width="11.85546875" style="1" customWidth="1"/>
+    <col min="105" max="105" width="17.7109375" style="1" customWidth="1"/>
+    <col min="106" max="106" width="11.85546875" style="1" customWidth="1"/>
+    <col min="107" max="107" width="17.7109375" style="1" customWidth="1"/>
+    <col min="108" max="108" width="14.85546875" style="1" customWidth="1"/>
+    <col min="109" max="109" width="17.7109375" style="1" customWidth="1"/>
+    <col min="110" max="110" width="12.28515625" style="1" customWidth="1"/>
+    <col min="111" max="111" width="17.7109375" style="1" customWidth="1"/>
+    <col min="112" max="112" width="9.140625" style="1"/>
+    <col min="113" max="113" width="17.7109375" style="1" customWidth="1"/>
+    <col min="114" max="114" width="9.140625" style="1"/>
+    <col min="115" max="115" width="17.7109375" style="1" customWidth="1"/>
+    <col min="116" max="116" width="18.42578125" style="1" customWidth="1"/>
+    <col min="117" max="117" width="17.7109375" style="1" customWidth="1"/>
+    <col min="118" max="118" width="10.140625" style="1" customWidth="1"/>
+    <col min="119" max="119" width="17.7109375" style="1" customWidth="1"/>
+    <col min="120" max="1107" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:119" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:103" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:119" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -2129,76 +2240,76 @@
         <v>1</v>
       </c>
       <c r="BH2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BR2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BV2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BI2" s="19" t="s">
+      <c r="BY2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BJ2" s="19" t="s">
+      <c r="BZ2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BK2" s="19" t="s">
+      <c r="CA2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BL2" s="19" t="s">
+      <c r="CB2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BM2" s="19" t="s">
+      <c r="CC2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BN2" s="19" t="s">
+      <c r="CD2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BO2" s="19" t="s">
+      <c r="CE2" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="BP2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BQ2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BS2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BT2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BU2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BV2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BW2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BX2" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="BY2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="BZ2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CA2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CB2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CC2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CD2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CE2" s="29" t="s">
-        <v>68</v>
       </c>
       <c r="CF2" s="29" t="s">
         <v>68</v>
@@ -2224,7 +2335,7 @@
       <c r="CM2" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="CN2" s="30" t="s">
+      <c r="CN2" s="28" t="s">
         <v>68</v>
       </c>
       <c r="CO2" s="29" t="s">
@@ -2260,8 +2371,56 @@
       <c r="CY2" s="29" t="s">
         <v>68</v>
       </c>
+      <c r="CZ2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DA2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DB2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DC2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DD2" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="DE2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DF2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DG2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DH2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DI2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DJ2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DK2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DL2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DM2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DN2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="DO2" s="29" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="3" spans="1:103" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:119" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>71</v>
       </c>
@@ -2269,7 +2428,7 @@
         <v>101</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>109</v>
@@ -2333,10 +2492,10 @@
         <v>39</v>
       </c>
       <c r="Y3" s="49" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Z3" s="49" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AA3" s="54" t="s">
         <v>97</v>
@@ -2366,211 +2525,259 @@
         <v>82</v>
       </c>
       <c r="AJ3" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK3" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL3" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="AM3" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="AN3" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="AO3" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP3" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="AQ3" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="AR3" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="AS3" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="AT3" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="AU3" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="AV3" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="AW3" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="AX3" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="AY3" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="AZ3" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="BA3" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="BB3" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC3" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="BD3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="AK3" s="27" t="s">
+      <c r="BE3" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="AL3" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="AM3" s="27" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN3" s="27" t="s">
+      <c r="BF3" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="BG3" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="BH3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="AO3" s="27" t="s">
+      <c r="BI3" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="AP3" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="AQ3" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="AR3" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="AS3" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="AT3" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="AU3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="AV3" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="AW3" s="27" t="s">
+      <c r="BJ3" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="BK3" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="BL3" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="BM3" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="AX3" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="AY3" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="AZ3" s="27" t="s">
+      <c r="BN3" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="BO3" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="BA3" s="27" t="s">
+      <c r="BP3" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="BB3" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="BC3" s="27" t="s">
-        <v>299</v>
-      </c>
-      <c r="BD3" s="27" t="s">
+      <c r="BQ3" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="BR3" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="BS3" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="BE3" s="27" t="s">
+      <c r="BT3" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="BF3" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="BG3" s="27" t="s">
+      <c r="BU3" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="BV3" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="BW3" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="BX3" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="BY3" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="BZ3" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="CA3" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="BH3" s="27" t="s">
+      <c r="CB3" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="BI3" s="27" t="s">
+      <c r="CC3" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="BJ3" s="27" t="s">
+      <c r="CD3" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="BK3" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="BL3" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="BM3" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="BN3" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="BO3" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="BP3" s="26" t="s">
+      <c r="CE3" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="CF3" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="BQ3" s="59" t="s">
-        <v>254</v>
-      </c>
-      <c r="BR3" s="26" t="s">
+      <c r="CG3" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="CH3" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="BS3" s="59" t="s">
-        <v>252</v>
-      </c>
-      <c r="BT3" s="26" t="s">
+      <c r="CI3" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="CJ3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="BU3" s="59" t="s">
-        <v>250</v>
-      </c>
-      <c r="BV3" s="26" t="s">
+      <c r="CK3" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="CL3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="BW3" s="59" t="s">
-        <v>248</v>
-      </c>
-      <c r="BX3" s="26" t="s">
+      <c r="CM3" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="CN3" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="BY3" s="59" t="s">
-        <v>246</v>
-      </c>
-      <c r="BZ3" s="26" t="s">
+      <c r="CO3" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="CP3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="CA3" s="59" t="s">
-        <v>244</v>
-      </c>
-      <c r="CB3" s="26" t="s">
+      <c r="CQ3" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="CR3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="CC3" s="59" t="s">
-        <v>242</v>
-      </c>
-      <c r="CD3" s="26" t="s">
+      <c r="CS3" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="CT3" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="CE3" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="CF3" s="26" t="s">
+      <c r="CU3" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="CV3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="CG3" s="59" t="s">
-        <v>239</v>
-      </c>
-      <c r="CH3" s="26" t="s">
+      <c r="CW3" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="CX3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="CI3" s="59" t="s">
-        <v>236</v>
-      </c>
-      <c r="CJ3" s="26" t="s">
+      <c r="CY3" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="CZ3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="CK3" s="59" t="s">
-        <v>234</v>
-      </c>
-      <c r="CL3" s="26" t="s">
+      <c r="DA3" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="DB3" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="CM3" s="59" t="s">
-        <v>232</v>
-      </c>
-      <c r="CN3" s="26" t="s">
+      <c r="DC3" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="DD3" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="CO3" s="59" t="s">
-        <v>230</v>
-      </c>
-      <c r="CP3" s="26" t="s">
+      <c r="DE3" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="DF3" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="CQ3" s="59" t="s">
-        <v>229</v>
-      </c>
-      <c r="CR3" s="26" t="s">
+      <c r="DG3" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="DH3" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="CS3" s="59" t="s">
-        <v>225</v>
-      </c>
-      <c r="CT3" s="26" t="s">
+      <c r="DI3" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="DJ3" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="CU3" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="CV3" s="26" t="s">
+      <c r="DK3" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="DL3" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="CW3" s="59" t="s">
-        <v>222</v>
-      </c>
-      <c r="CX3" s="26" t="s">
+      <c r="DM3" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="DN3" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="CY3" s="59" t="s">
-        <v>220</v>
+      <c r="DO3" s="59" t="s">
+        <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:103" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:119" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
@@ -2596,7 +2803,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J4" s="38" t="s">
         <v>123</v>
@@ -2644,7 +2851,7 @@
         <v>40</v>
       </c>
       <c r="Y4" s="38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Z4" s="38" t="s">
         <v>9</v>
@@ -2674,214 +2881,262 @@
         <v>45</v>
       </c>
       <c r="AI4" s="38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AJ4" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="AK4" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="AL4" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="AM4" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="AN4" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="AO4" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="AP4" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="AQ4" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="AR4" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS4" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="AT4" s="38" t="s">
+        <v>290</v>
+      </c>
+      <c r="AU4" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="AV4" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="AW4" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="AX4" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="AY4" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="AZ4" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="BA4" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="BB4" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="BC4" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="BD4" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="BE4" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="AK4" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="AL4" s="38" t="s">
-        <v>275</v>
-      </c>
-      <c r="AM4" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="AN4" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="AO4" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="AP4" s="38" t="s">
-        <v>289</v>
-      </c>
-      <c r="AQ4" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="AR4" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="AS4" s="38" t="s">
+      <c r="BF4" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="BG4" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="BH4" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="BI4" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="BJ4" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="BK4" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="BL4" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="AT4" s="38" t="s">
-        <v>292</v>
-      </c>
-      <c r="AU4" s="38" t="s">
+      <c r="BM4" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="AV4" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="AW4" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX4" s="38" t="s">
-        <v>296</v>
-      </c>
-      <c r="AY4" s="38" t="s">
-        <v>210</v>
-      </c>
-      <c r="AZ4" s="38" t="s">
+      <c r="BN4" s="38" t="s">
+        <v>297</v>
+      </c>
+      <c r="BO4" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="BA4" s="38" t="s">
+      <c r="BP4" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="BB4" s="38" t="s">
-        <v>301</v>
-      </c>
-      <c r="BC4" s="38" t="s">
+      <c r="BQ4" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="BR4" s="38" t="s">
+        <v>298</v>
+      </c>
+      <c r="BS4" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="BD4" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="BE4" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="BF4" s="38" t="s">
-        <v>302</v>
-      </c>
-      <c r="BG4" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="BH4" s="38" t="s">
+      <c r="BT4" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="BU4" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="BV4" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="BW4" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="BX4" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="BI4" s="38" t="s">
+      <c r="BY4" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="BJ4" s="38" t="s">
+      <c r="BZ4" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="BK4" s="38" t="s">
+      <c r="CA4" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="BL4" s="38" t="s">
+      <c r="CB4" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="BM4" s="38" t="s">
+      <c r="CC4" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="BN4" s="38" t="s">
+      <c r="CD4" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="BO4" s="38" t="s">
+      <c r="CE4" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="BP4" s="38" t="s">
+      <c r="CF4" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="BQ4" s="38" t="s">
+      <c r="CG4" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="CH4" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="CI4" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="CJ4" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="CK4" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="BR4" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS4" s="38" t="s">
+      <c r="CL4" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="CM4" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="BT4" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="BU4" s="38" t="s">
+      <c r="CN4" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="CO4" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="BV4" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="BW4" s="38" t="s">
+      <c r="CP4" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="CQ4" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="BX4" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="BY4" s="38" t="s">
+      <c r="CR4" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="CS4" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="BZ4" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="CA4" s="38" t="s">
+      <c r="CT4" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="CU4" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="CB4" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="CC4" s="38" t="s">
+      <c r="CV4" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="CW4" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="CD4" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="CE4" s="38" t="s">
+      <c r="CX4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="CY4" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="CF4" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="CG4" s="38" t="s">
+      <c r="CZ4" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="DA4" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="CH4" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="CI4" s="38" t="s">
+      <c r="DB4" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="DC4" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="CJ4" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="CK4" s="38" t="s">
+      <c r="DD4" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="DE4" s="38" t="s">
         <v>266</v>
       </c>
-      <c r="CL4" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="CM4" s="38" t="s">
+      <c r="DF4" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="DG4" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="CN4" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="CO4" s="38" t="s">
+      <c r="DH4" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="DI4" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="CP4" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="CQ4" s="38" t="s">
+      <c r="DJ4" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="DK4" s="38" t="s">
         <v>269</v>
       </c>
-      <c r="CR4" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="CS4" s="38" t="s">
+      <c r="DL4" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="DM4" s="41" t="s">
         <v>270</v>
       </c>
-      <c r="CT4" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="CU4" s="38" t="s">
+      <c r="DN4" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="DO4" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="CV4" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="CW4" s="41" t="s">
-        <v>272</v>
-      </c>
-      <c r="CX4" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="CY4" s="38" t="s">
-        <v>273</v>
-      </c>
     </row>
-    <row r="5" spans="1:103" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:119" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>70</v>
       </c>
@@ -2907,7 +3162,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>167</v>
@@ -2955,7 +3210,7 @@
         <v>4</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>32</v>
@@ -2988,212 +3243,260 @@
         <v>47</v>
       </c>
       <c r="AJ5" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="AO5" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="AN5" s="4" t="s">
+      <c r="AP5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AR5" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AS5" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AT5" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="AQ5" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="AR5" s="4" t="s">
+      <c r="AU5" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="AS5" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="AT5" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="AU5" s="4" t="s">
+      <c r="AV5" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="BA5" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="BF5" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="BG5" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="BH5" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI5" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="BJ5" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="BK5" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="BL5" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="BM5" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="BN5" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="BO5" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="BP5" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ5" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="BR5" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="BS5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="AV5" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="AW5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="AX5" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AY5" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="AZ5" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="BA5" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="BB5" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="BC5" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="BE5" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="BH5" s="4" t="s">
+      <c r="BT5" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="BU5" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="BV5" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="BW5" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="BX5" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="BI5" s="4" t="s">
+      <c r="BY5" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="BJ5" s="4" t="s">
+      <c r="BZ5" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="BK5" s="4" t="s">
+      <c r="CA5" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="BL5" s="4" t="s">
+      <c r="CB5" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="BM5" s="4" t="s">
+      <c r="CC5" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="BN5" s="4" t="s">
+      <c r="CD5" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="BO5" s="4" t="s">
+      <c r="CE5" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="BP5" s="4" t="s">
+      <c r="CF5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BQ5" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="BR5" s="4" t="s">
+      <c r="CG5" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="CH5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BS5" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="BT5" s="7" t="s">
+      <c r="CI5" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="CJ5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BU5" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="BV5" s="4" t="s">
+      <c r="CK5" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="CL5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BW5" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="BX5" s="4" t="s">
+      <c r="CM5" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="CN5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BY5" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="BZ5" s="7" t="s">
+      <c r="CO5" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="CP5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="CA5" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="CB5" s="7" t="s">
+      <c r="CQ5" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="CR5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="CC5" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="CD5" s="7" t="s">
+      <c r="CS5" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="CT5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="CE5" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="CF5" s="7" t="s">
+      <c r="CU5" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="CV5" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="CG5" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="CH5" s="4" t="s">
+      <c r="CW5" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="CX5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="CI5" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="CJ5" s="4" t="s">
+      <c r="CY5" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="CZ5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="CK5" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="CL5" s="4" t="s">
+      <c r="DA5" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="DB5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="CM5" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="CN5" s="14" t="s">
+      <c r="DC5" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="DD5" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="CO5" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="CP5" s="4" t="s">
+      <c r="DE5" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="DF5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="CQ5" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="CR5" s="7" t="s">
+      <c r="DG5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="DH5" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="CS5" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="CT5" s="4" t="s">
+      <c r="DI5" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="DJ5" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CU5" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="CV5" s="7" t="s">
+      <c r="DK5" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="DL5" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="CW5" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="CX5" s="7" t="s">
+      <c r="DM5" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="DN5" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="CY5" s="4" t="s">
-        <v>221</v>
+      <c r="DO5" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:103" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:119" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:119" x14ac:dyDescent="0.25">
       <c r="G7" s="32"/>
     </row>
   </sheetData>
@@ -3211,7 +3514,7 @@
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 CW6:CW1048576 CU6:CU1048576 CY6:CY1048576 CS6:CS1048576 CQ6:CQ1048576 CO6:CO1048576 CM6:CM1048576 CK6:CK1048576 CI6:CI1048576 CG6:CG1048576 CE6:CE1048576 CC6:CC1048576 CA6:CA1048576 BY6:BY1048576 BW6:BW1048576 BU6:BU1048576 BS6:BS1048576 BQ6:BQ1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 DM6:DM1048576 DK6:DK1048576 DO6:DO1048576 DI6:DI1048576 DG6:DG1048576 DE6:DE1048576 DC6:DC1048576 DA6:DA1048576 CY6:CY1048576 CW6:CW1048576 CU6:CU1048576 CS6:CS1048576 CQ6:CQ1048576 CO6:CO1048576 CM6:CM1048576 CK6:CK1048576 CI6:CI1048576 CG6:CG1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3224,7 +3527,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AL6:AL1048576 AP6:AP1048576 AX6:AX1048576 BB6:BB1048576 BF6:BF1048576 AT6:AT1048576</xm:sqref>
+          <xm:sqref>AL6:AL1048576 AP6:AP1048576 BF6:BF1048576 AT6:AT1048576 BR6:BR1048576 BJ6:BJ1048576 BN6:BN1048576 BV6:BV1048576 AX6:AX1048576 BB6:BB1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3307,17 +3610,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added another date block plus suppport for more
</commit_message>
<xml_diff>
--- a/templates/extended_aspace_import_excel_template.xlsx
+++ b/templates/extended_aspace_import_excel_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbi\Documents\aspace\archivesspace\plugins\aspace-import-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA5EF00-85EB-46C3-9BA1-7941A4081E69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FE0F62-F18D-42EA-84C0-796E4FC6A812}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="780" windowWidth="20085" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="355">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -108,15 +108,6 @@
     <t>end</t>
   </si>
   <si>
-    <t>Date Begin</t>
-  </si>
-  <si>
-    <t>Date end</t>
-  </si>
-  <si>
-    <t>Dates Type</t>
-  </si>
-  <si>
     <t>Extent type: cubic feet, cds, etc.</t>
   </si>
   <si>
@@ -366,9 +357,6 @@
     <t>Extent portion</t>
   </si>
   <si>
-    <t>Date Certainty</t>
-  </si>
-  <si>
     <t>Date certainty (CONTROLLED LIST; Default: blank)</t>
   </si>
   <si>
@@ -529,9 +517,6 @@
   </si>
   <si>
     <t>Restrictions Apply?</t>
-  </si>
-  <si>
-    <t>Dates Label</t>
   </si>
   <si>
     <t>Hierarchical relationship of new component to context object. 1=the first level of archival objects, 2=second level, 3=third level, etc. 
@@ -658,9 +643,6 @@
     <t>families_agent_relator_1</t>
   </si>
   <si>
-    <t>This is the template for importing using aspace-import-excel.  You may replace this line with something of your choosing after you've copied the file for your use.</t>
-  </si>
-  <si>
     <t>instance type: Accession, Audio, Books, etc.</t>
   </si>
   <si>
@@ -1055,6 +1037,63 @@
   </si>
   <si>
     <t>Agent(5) Relator</t>
+  </si>
+  <si>
+    <t>Date(1) Label</t>
+  </si>
+  <si>
+    <t>Date(1) Begin</t>
+  </si>
+  <si>
+    <t>Date(1) end</t>
+  </si>
+  <si>
+    <t>Date(1) Type</t>
+  </si>
+  <si>
+    <t>Date(1) expression</t>
+  </si>
+  <si>
+    <t>Date(1) Certainty</t>
+  </si>
+  <si>
+    <t>dates_label_2</t>
+  </si>
+  <si>
+    <t>Date(2) Label</t>
+  </si>
+  <si>
+    <t>Date(2) Begin</t>
+  </si>
+  <si>
+    <t>begin_2</t>
+  </si>
+  <si>
+    <t>end_2</t>
+  </si>
+  <si>
+    <t>Date(2) end</t>
+  </si>
+  <si>
+    <t>date_type_2</t>
+  </si>
+  <si>
+    <t>Date(2) Type</t>
+  </si>
+  <si>
+    <t>expression_2</t>
+  </si>
+  <si>
+    <t>Date(2) expression</t>
+  </si>
+  <si>
+    <t>date_certainty_2</t>
+  </si>
+  <si>
+    <t>Date(2) Certainty</t>
+  </si>
+  <si>
+    <t>This is the expanded template for importing using aspace-import-excel.  You may replace this line with something of your choosing after you've copied the file for your use.</t>
   </si>
 </sst>
 </file>
@@ -1943,7 +1982,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:APO7"/>
+  <dimension ref="A1:APU7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -1968,222 +2007,228 @@
     <col min="14" max="14" width="11" style="50" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" style="50" customWidth="1"/>
     <col min="16" max="16" width="23.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" style="1" customWidth="1"/>
-    <col min="18" max="25" width="26.85546875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="23" style="1"/>
-    <col min="27" max="27" width="23" style="50"/>
-    <col min="28" max="28" width="10.42578125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="19" style="50" customWidth="1"/>
-    <col min="30" max="30" width="19.140625" style="50" customWidth="1"/>
-    <col min="31" max="31" width="10.42578125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="50" customWidth="1"/>
-    <col min="33" max="33" width="10.42578125" style="1" customWidth="1"/>
-    <col min="34" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="15.28515625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="22.7109375" style="1"/>
-    <col min="38" max="38" width="15.28515625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="13" style="1" customWidth="1"/>
-    <col min="40" max="40" width="15.42578125" style="1" customWidth="1"/>
-    <col min="41" max="41" width="22.7109375" style="1"/>
+    <col min="17" max="17" width="15.140625" style="50" customWidth="1"/>
+    <col min="18" max="18" width="26.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="50" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" style="50" customWidth="1"/>
+    <col min="22" max="22" width="23.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" style="50" customWidth="1"/>
+    <col min="24" max="31" width="26.85546875" style="1" customWidth="1"/>
+    <col min="32" max="32" width="23" style="1"/>
+    <col min="33" max="33" width="23" style="50"/>
+    <col min="34" max="34" width="10.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="19" style="50" customWidth="1"/>
+    <col min="36" max="36" width="19.140625" style="50" customWidth="1"/>
+    <col min="37" max="37" width="10.42578125" style="1" customWidth="1"/>
+    <col min="38" max="38" width="11.42578125" style="50" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" style="1" customWidth="1"/>
+    <col min="40" max="41" width="9.140625" style="1"/>
     <col min="42" max="42" width="15.28515625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="9.140625" style="1"/>
-    <col min="44" max="44" width="15.140625" style="1" customWidth="1"/>
-    <col min="45" max="45" width="20.140625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="15.28515625" style="1" customWidth="1"/>
-    <col min="47" max="47" width="12.85546875" style="1" customWidth="1"/>
-    <col min="48" max="48" width="15.140625" style="1" customWidth="1"/>
-    <col min="49" max="49" width="20.140625" style="1" customWidth="1"/>
-    <col min="50" max="50" width="15.28515625" style="1" customWidth="1"/>
-    <col min="51" max="51" width="12.85546875" style="1" customWidth="1"/>
-    <col min="52" max="52" width="15.140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="20.140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="15.28515625" style="1" customWidth="1"/>
-    <col min="55" max="55" width="12.85546875" style="1" customWidth="1"/>
-    <col min="56" max="56" width="9.140625" style="1"/>
-    <col min="57" max="57" width="11.42578125" style="1" customWidth="1"/>
-    <col min="58" max="58" width="15.28515625" style="1" customWidth="1"/>
-    <col min="59" max="60" width="9.140625" style="1"/>
-    <col min="61" max="61" width="11.42578125" style="1" customWidth="1"/>
-    <col min="62" max="62" width="15.28515625" style="1" customWidth="1"/>
-    <col min="63" max="65" width="9.140625" style="1"/>
-    <col min="66" max="66" width="15.28515625" style="1" customWidth="1"/>
-    <col min="67" max="69" width="9.140625" style="1"/>
-    <col min="70" max="70" width="15.28515625" style="1" customWidth="1"/>
-    <col min="71" max="73" width="9.140625" style="1"/>
-    <col min="74" max="74" width="15.28515625" style="1" customWidth="1"/>
-    <col min="75" max="75" width="9.140625" style="1"/>
-    <col min="76" max="76" width="11.5703125" style="1" customWidth="1"/>
-    <col min="77" max="77" width="12.28515625" style="1" customWidth="1"/>
-    <col min="78" max="80" width="13.5703125" style="1" customWidth="1"/>
-    <col min="81" max="82" width="10.85546875" style="1" customWidth="1"/>
-    <col min="83" max="83" width="15.42578125" style="1" customWidth="1"/>
-    <col min="84" max="84" width="9.28515625" style="1"/>
-    <col min="85" max="85" width="17.7109375" style="1" customWidth="1"/>
-    <col min="86" max="86" width="17" style="1" customWidth="1"/>
-    <col min="87" max="87" width="17.7109375" style="1" customWidth="1"/>
-    <col min="88" max="88" width="12.28515625" style="1" customWidth="1"/>
-    <col min="89" max="89" width="17.7109375" style="1" customWidth="1"/>
-    <col min="90" max="90" width="11.7109375" style="1" customWidth="1"/>
+    <col min="43" max="43" width="22.7109375" style="1"/>
+    <col min="44" max="44" width="15.28515625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="13" style="1" customWidth="1"/>
+    <col min="46" max="46" width="15.42578125" style="1" customWidth="1"/>
+    <col min="47" max="47" width="22.7109375" style="1"/>
+    <col min="48" max="48" width="15.28515625" style="1" customWidth="1"/>
+    <col min="49" max="49" width="9.140625" style="1"/>
+    <col min="50" max="50" width="15.140625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="20.140625" style="1" customWidth="1"/>
+    <col min="52" max="52" width="15.28515625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="12.85546875" style="1" customWidth="1"/>
+    <col min="54" max="54" width="15.140625" style="1" customWidth="1"/>
+    <col min="55" max="55" width="20.140625" style="1" customWidth="1"/>
+    <col min="56" max="56" width="15.28515625" style="1" customWidth="1"/>
+    <col min="57" max="57" width="12.85546875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="15.140625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="20.140625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="15.28515625" style="1" customWidth="1"/>
+    <col min="61" max="61" width="12.85546875" style="1" customWidth="1"/>
+    <col min="62" max="62" width="9.140625" style="1"/>
+    <col min="63" max="63" width="11.42578125" style="1" customWidth="1"/>
+    <col min="64" max="64" width="15.28515625" style="1" customWidth="1"/>
+    <col min="65" max="66" width="9.140625" style="1"/>
+    <col min="67" max="67" width="11.42578125" style="1" customWidth="1"/>
+    <col min="68" max="68" width="15.28515625" style="1" customWidth="1"/>
+    <col min="69" max="71" width="9.140625" style="1"/>
+    <col min="72" max="72" width="15.28515625" style="1" customWidth="1"/>
+    <col min="73" max="75" width="9.140625" style="1"/>
+    <col min="76" max="76" width="15.28515625" style="1" customWidth="1"/>
+    <col min="77" max="79" width="9.140625" style="1"/>
+    <col min="80" max="80" width="15.28515625" style="1" customWidth="1"/>
+    <col min="81" max="81" width="9.140625" style="1"/>
+    <col min="82" max="82" width="11.5703125" style="1" customWidth="1"/>
+    <col min="83" max="83" width="12.28515625" style="1" customWidth="1"/>
+    <col min="84" max="86" width="13.5703125" style="1" customWidth="1"/>
+    <col min="87" max="88" width="10.85546875" style="1" customWidth="1"/>
+    <col min="89" max="89" width="15.42578125" style="1" customWidth="1"/>
+    <col min="90" max="90" width="9.28515625" style="1"/>
     <col min="91" max="91" width="17.7109375" style="1" customWidth="1"/>
-    <col min="92" max="92" width="16" style="1" customWidth="1"/>
+    <col min="92" max="92" width="17" style="1" customWidth="1"/>
     <col min="93" max="93" width="17.7109375" style="1" customWidth="1"/>
-    <col min="94" max="94" width="9.140625" style="1"/>
+    <col min="94" max="94" width="12.28515625" style="1" customWidth="1"/>
     <col min="95" max="95" width="17.7109375" style="1" customWidth="1"/>
-    <col min="96" max="96" width="12" customWidth="1"/>
+    <col min="96" max="96" width="11.7109375" style="1" customWidth="1"/>
     <col min="97" max="97" width="17.7109375" style="1" customWidth="1"/>
-    <col min="98" max="98" width="11.85546875" style="1" customWidth="1"/>
+    <col min="98" max="98" width="16" style="1" customWidth="1"/>
     <col min="99" max="99" width="17.7109375" style="1" customWidth="1"/>
-    <col min="100" max="100" width="11.85546875" style="1" customWidth="1"/>
+    <col min="100" max="100" width="9.140625" style="1"/>
     <col min="101" max="101" width="17.7109375" style="1" customWidth="1"/>
-    <col min="102" max="102" width="11.85546875" style="1" customWidth="1"/>
+    <col min="102" max="102" width="12" customWidth="1"/>
     <col min="103" max="103" width="17.7109375" style="1" customWidth="1"/>
     <col min="104" max="104" width="11.85546875" style="1" customWidth="1"/>
     <col min="105" max="105" width="17.7109375" style="1" customWidth="1"/>
     <col min="106" max="106" width="11.85546875" style="1" customWidth="1"/>
     <col min="107" max="107" width="17.7109375" style="1" customWidth="1"/>
-    <col min="108" max="108" width="14.85546875" style="1" customWidth="1"/>
+    <col min="108" max="108" width="11.85546875" style="1" customWidth="1"/>
     <col min="109" max="109" width="17.7109375" style="1" customWidth="1"/>
-    <col min="110" max="110" width="12.28515625" style="1" customWidth="1"/>
+    <col min="110" max="110" width="11.85546875" style="1" customWidth="1"/>
     <col min="111" max="111" width="17.7109375" style="1" customWidth="1"/>
-    <col min="112" max="112" width="9.140625" style="1"/>
+    <col min="112" max="112" width="11.85546875" style="1" customWidth="1"/>
     <col min="113" max="113" width="17.7109375" style="1" customWidth="1"/>
-    <col min="114" max="114" width="9.140625" style="1"/>
+    <col min="114" max="114" width="14.85546875" style="1" customWidth="1"/>
     <col min="115" max="115" width="17.7109375" style="1" customWidth="1"/>
-    <col min="116" max="116" width="18.42578125" style="1" customWidth="1"/>
+    <col min="116" max="116" width="12.28515625" style="1" customWidth="1"/>
     <col min="117" max="117" width="17.7109375" style="1" customWidth="1"/>
-    <col min="118" max="118" width="10.140625" style="1" customWidth="1"/>
+    <col min="118" max="118" width="9.140625" style="1"/>
     <col min="119" max="119" width="17.7109375" style="1" customWidth="1"/>
-    <col min="120" max="1107" width="9.28515625" style="1"/>
+    <col min="120" max="120" width="9.140625" style="1"/>
+    <col min="121" max="121" width="17.7109375" style="1" customWidth="1"/>
+    <col min="122" max="122" width="18.42578125" style="1" customWidth="1"/>
+    <col min="123" max="123" width="17.7109375" style="1" customWidth="1"/>
+    <col min="124" max="124" width="10.140625" style="1" customWidth="1"/>
+    <col min="125" max="125" width="17.7109375" style="1" customWidth="1"/>
+    <col min="126" max="1113" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:125" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>209</v>
+        <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:119" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:125" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K2" s="42" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N2" s="55" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O2" s="55" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="Q2" s="55" t="s">
+        <v>96</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC2" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD2" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF2" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="19" t="s">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="U2" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO2" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="AP2" s="48" t="s">
         <v>1</v>
@@ -2191,266 +2236,284 @@
       <c r="AQ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AR2" s="19" t="s">
+      <c r="AR2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="AS2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AT2" s="48" t="s">
+      <c r="AT2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="AU2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AV2" s="19" t="s">
+      <c r="AV2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="AW2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AX2" s="48" t="s">
+      <c r="AX2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="AY2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AZ2" s="19" t="s">
+      <c r="AZ2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BA2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BB2" s="48" t="s">
+      <c r="BB2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BC2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BD2" s="19" t="s">
+      <c r="BD2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BE2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BF2" s="48" t="s">
+      <c r="BF2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BG2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BH2" s="19" t="s">
+      <c r="BH2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BI2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BJ2" s="48" t="s">
+      <c r="BJ2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BK2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BL2" s="19" t="s">
+      <c r="BL2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BM2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BN2" s="48" t="s">
+      <c r="BN2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BO2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BP2" s="19" t="s">
+      <c r="BP2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BQ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BR2" s="48" t="s">
+      <c r="BR2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BS2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BT2" s="19" t="s">
+      <c r="BT2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BU2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BV2" s="48" t="s">
+      <c r="BV2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BW2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BX2" s="19" t="s">
-        <v>124</v>
+      <c r="BX2" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="BY2" s="19" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="BZ2" s="19" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="CA2" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="CB2" s="19" t="s">
-        <v>124</v>
+        <v>1</v>
+      </c>
+      <c r="CB2" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="CC2" s="19" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="CD2" s="19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="CE2" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="CF2" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="CF2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="CG2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="CH2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="CI2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="CJ2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="CK2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="CL2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CM2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CN2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CO2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CP2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CQ2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CR2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CS2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CT2" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="CU2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CV2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CW2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CX2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CY2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="CZ2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DA2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DB2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DC2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DD2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DE2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DF2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DG2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DH2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DI2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DJ2" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="DK2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DL2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DM2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DN2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DO2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DP2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DQ2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DR2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DS2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DT2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DU2" s="29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:125" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="CG2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CH2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CI2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CJ2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CK2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CL2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CM2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CN2" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="CO2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CP2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CQ2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CR2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CS2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CT2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CU2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CV2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CW2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CX2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CY2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="CZ2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DA2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DB2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DC2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DD2" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="DE2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DF2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DG2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DH2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DI2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DJ2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DK2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DL2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DM2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DN2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="DO2" s="29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:119" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
-        <v>71</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K3" s="43" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>2</v>
@@ -2465,319 +2528,337 @@
         <v>18</v>
       </c>
       <c r="P3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="W3" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF3" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="AG3" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI3" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ3" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL3" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="X3" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y3" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z3" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA3" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC3" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD3" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF3" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="AG3" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH3" s="25" t="s">
+      <c r="AN3" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO3" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="AI3" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ3" s="27" t="s">
+      <c r="AP3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="AQ3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="AR3" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="AS3" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="AT3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="AU3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV3" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="AW3" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="AX3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="AZ3" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="BA3" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="BB3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="BC3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="BD3" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="BE3" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="BF3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="BG3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="BH3" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="BI3" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="BJ3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="BK3" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="BL3" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="BM3" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="BN3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="BO3" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="BP3" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="BQ3" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="BR3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="AK3" s="27" t="s">
+      <c r="BS3" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="BT3" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="BU3" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="BV3" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="BW3" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX3" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="BY3" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="BZ3" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="CA3" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="CB3" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="CC3" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="CD3" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="CE3" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="CF3" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="CG3" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="AL3" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="AM3" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="AN3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="AO3" s="27" t="s">
+      <c r="CH3" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="CI3" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="CJ3" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="CK3" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="AP3" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="AQ3" s="27" t="s">
-        <v>301</v>
-      </c>
-      <c r="AR3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="AS3" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="AT3" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="AU3" s="27" t="s">
-        <v>325</v>
-      </c>
-      <c r="AV3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="AW3" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="AX3" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="AY3" s="27" t="s">
-        <v>325</v>
-      </c>
-      <c r="AZ3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="BA3" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="BB3" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="BC3" s="27" t="s">
-        <v>325</v>
-      </c>
-      <c r="BD3" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="BE3" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="BF3" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="BG3" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="BH3" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="BI3" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="BJ3" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="BK3" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="BL3" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="BM3" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="BN3" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="BO3" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="BP3" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="BQ3" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="BR3" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="BS3" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="BT3" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="BU3" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="BV3" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="BW3" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="BX3" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="BY3" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="BZ3" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="CA3" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="CB3" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="CC3" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="CD3" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="CE3" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="CF3" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="CG3" s="59" t="s">
-        <v>252</v>
-      </c>
-      <c r="CH3" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="CI3" s="59" t="s">
-        <v>250</v>
-      </c>
-      <c r="CJ3" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="CK3" s="59" t="s">
-        <v>248</v>
-      </c>
       <c r="CL3" s="26" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="CM3" s="59" t="s">
         <v>246</v>
       </c>
       <c r="CN3" s="26" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="CO3" s="59" t="s">
         <v>244</v>
       </c>
       <c r="CP3" s="26" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="CQ3" s="59" t="s">
         <v>242</v>
       </c>
       <c r="CR3" s="26" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="CS3" s="59" t="s">
         <v>240</v>
       </c>
       <c r="CT3" s="26" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="CU3" s="59" t="s">
         <v>238</v>
       </c>
       <c r="CV3" s="26" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="CW3" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="CX3" s="26" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="CY3" s="59" t="s">
         <v>234</v>
       </c>
       <c r="CZ3" s="26" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="DA3" s="59" t="s">
         <v>232</v>
       </c>
       <c r="DB3" s="26" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="DC3" s="59" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="DD3" s="26" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="DE3" s="59" t="s">
         <v>228</v>
       </c>
       <c r="DF3" s="26" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="DG3" s="59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DH3" s="26" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="DI3" s="59" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="DJ3" s="26" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="DK3" s="59" t="s">
         <v>222</v>
       </c>
       <c r="DL3" s="26" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="DM3" s="59" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="DN3" s="26" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="DO3" s="59" t="s">
-        <v>218</v>
+        <v>217</v>
+      </c>
+      <c r="DP3" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="DQ3" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="DR3" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="DS3" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="DT3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="DU3" s="59" t="s">
+        <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:119" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:125" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
@@ -2785,37 +2866,37 @@
         <v>6</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H4" s="38" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K4" s="44" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="L4" s="38" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N4" s="40" t="s">
         <v>26</v>
@@ -2826,677 +2907,713 @@
       <c r="P4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="38" t="s">
+      <c r="Q4" s="40" t="s">
         <v>25</v>
       </c>
       <c r="R4" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="T4" s="40" t="s">
+        <v>345</v>
+      </c>
+      <c r="U4" s="40" t="s">
+        <v>346</v>
+      </c>
+      <c r="V4" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="W4" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="X4" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="Y4" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z4" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA4" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB4" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC4" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD4" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE4" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF4" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG4" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH4" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI4" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ4" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL4" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM4" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="S4" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="T4" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="U4" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="V4" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="W4" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="X4" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="38" t="s">
+      <c r="AN4" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO4" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="Z4" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA4" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB4" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC4" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD4" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE4" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF4" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG4" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH4" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI4" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="AJ4" s="38" t="s">
-        <v>205</v>
-      </c>
-      <c r="AK4" s="38" t="s">
+      <c r="AP4" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ4" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR4" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS4" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="AT4" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="AU4" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="AV4" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="AW4" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="AX4" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="AL4" s="38" t="s">
-        <v>273</v>
-      </c>
-      <c r="AM4" s="38" t="s">
+      <c r="AY4" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AN4" s="38" t="s">
+      <c r="AZ4" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="BA4" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="AO4" s="38" t="s">
+      <c r="BB4" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="BC4" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="BD4" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="BE4" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="BF4" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="BG4" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="BH4" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="BI4" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="BJ4" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="BK4" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="BL4" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="BM4" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN4" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="BO4" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="BP4" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="BQ4" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="BR4" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="AP4" s="38" t="s">
-        <v>287</v>
-      </c>
-      <c r="AQ4" s="38" t="s">
+      <c r="BS4" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="AR4" s="38" t="s">
+      <c r="BT4" s="38" t="s">
+        <v>291</v>
+      </c>
+      <c r="BU4" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="AS4" s="38" t="s">
+      <c r="BV4" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="AT4" s="38" t="s">
-        <v>290</v>
-      </c>
-      <c r="AU4" s="38" t="s">
+      <c r="BW4" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="BX4" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="BY4" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="AV4" s="38" t="s">
-        <v>326</v>
-      </c>
-      <c r="AW4" s="38" t="s">
-        <v>328</v>
-      </c>
-      <c r="AX4" s="38" t="s">
-        <v>330</v>
-      </c>
-      <c r="AY4" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="AZ4" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="BA4" s="38" t="s">
-        <v>336</v>
-      </c>
-      <c r="BB4" s="38" t="s">
-        <v>338</v>
-      </c>
-      <c r="BC4" s="38" t="s">
-        <v>340</v>
-      </c>
-      <c r="BD4" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="BE4" s="38" t="s">
-        <v>207</v>
-      </c>
-      <c r="BF4" s="38" t="s">
-        <v>293</v>
-      </c>
-      <c r="BG4" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="BH4" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="BI4" s="38" t="s">
-        <v>309</v>
-      </c>
-      <c r="BJ4" s="38" t="s">
+      <c r="BZ4" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="BK4" s="38" t="s">
+      <c r="CA4" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="BL4" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="BM4" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="BN4" s="38" t="s">
-        <v>297</v>
-      </c>
-      <c r="BO4" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="BP4" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="BQ4" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="BR4" s="38" t="s">
-        <v>298</v>
-      </c>
-      <c r="BS4" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="BT4" s="38" t="s">
+      <c r="CB4" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="CC4" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="BU4" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="BV4" s="38" t="s">
-        <v>321</v>
-      </c>
-      <c r="BW4" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="BX4" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="BY4" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="BZ4" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="CA4" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="CB4" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="CC4" s="38" t="s">
-        <v>129</v>
-      </c>
       <c r="CD4" s="38" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="CE4" s="38" t="s">
-        <v>176</v>
+        <v>123</v>
       </c>
       <c r="CF4" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="CG4" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="CH4" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="CI4" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="CJ4" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="CK4" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="CL4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="CM4" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="CN4" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="CO4" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="CP4" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="CQ4" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="CR4" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="CS4" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="CT4" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="CG4" s="38" t="s">
+      <c r="CU4" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="CV4" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="CW4" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="CX4" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="CY4" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="CH4" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="CI4" s="38" t="s">
+      <c r="CZ4" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="DA4" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="CJ4" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="CK4" s="38" t="s">
+      <c r="DB4" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="DC4" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="CL4" s="38" t="s">
+      <c r="DD4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="CM4" s="38" t="s">
+      <c r="DE4" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="CN4" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="CO4" s="38" t="s">
+      <c r="DF4" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="DG4" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="CP4" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="CQ4" s="38" t="s">
+      <c r="DH4" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="DI4" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="CR4" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="CS4" s="38" t="s">
+      <c r="DJ4" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK4" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="CT4" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="CU4" s="38" t="s">
+      <c r="DL4" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="DM4" s="38" t="s">
         <v>261</v>
-      </c>
-      <c r="CV4" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="CW4" s="38" t="s">
-        <v>262</v>
-      </c>
-      <c r="CX4" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="CY4" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="CZ4" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="DA4" s="38" t="s">
-        <v>264</v>
-      </c>
-      <c r="DB4" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="DC4" s="38" t="s">
-        <v>265</v>
-      </c>
-      <c r="DD4" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="DE4" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="DF4" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="DG4" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="DH4" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="DI4" s="38" t="s">
-        <v>268</v>
-      </c>
-      <c r="DJ4" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="DK4" s="38" t="s">
-        <v>269</v>
-      </c>
-      <c r="DL4" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="DM4" s="41" t="s">
-        <v>270</v>
       </c>
       <c r="DN4" s="41" t="s">
         <v>64</v>
       </c>
       <c r="DO4" s="38" t="s">
-        <v>271</v>
+        <v>262</v>
+      </c>
+      <c r="DP4" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="DQ4" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="DR4" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="DS4" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="DT4" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="DU4" s="38" t="s">
+        <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:119" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:125" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>169</v>
+        <v>336</v>
       </c>
       <c r="N5" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="O5" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q5" s="53" t="s">
+        <v>340</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="T5" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="U5" s="53" t="s">
+        <v>347</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="W5" s="53" t="s">
+        <v>351</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="53" t="s">
+      <c r="AB5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="S5" s="4" t="s">
+      <c r="AG5" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI5" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ5" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL5" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM5" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="T5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA5" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC5" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD5" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF5" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="BA5" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="AN5" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="AO5" s="4" t="s">
+      <c r="BB5" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="BF5" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="BG5" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="BH5" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="BI5" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="BJ5" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK5" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="BL5" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="BM5" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="BN5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="BO5" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="BP5" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="BQ5" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="BR5" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="BS5" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="BT5" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="BU5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="BV5" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="BW5" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="BX5" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="BY5" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="AP5" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="AS5" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="AT5" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="AW5" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="AX5" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="AY5" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="AZ5" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="BA5" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="BB5" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="BC5" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="BE5" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="BH5" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="BI5" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="BJ5" s="4" t="s">
+      <c r="BZ5" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="BK5" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="BL5" s="4" t="s">
+      <c r="CA5" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="BM5" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="BN5" s="4" t="s">
+      <c r="CB5" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="BO5" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="BP5" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="BQ5" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="BR5" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="BS5" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="BT5" s="4" t="s">
+      <c r="CC5" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="BU5" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="BV5" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="BW5" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="BX5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="BY5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="BZ5" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="CA5" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="CB5" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="CC5" s="4" t="s">
-        <v>133</v>
-      </c>
       <c r="CD5" s="4" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="CE5" s="4" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="CF5" s="4" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="CG5" s="4" t="s">
-        <v>253</v>
+        <v>175</v>
       </c>
       <c r="CH5" s="4" t="s">
-        <v>49</v>
+        <v>174</v>
       </c>
       <c r="CI5" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="CJ5" s="7" t="s">
-        <v>52</v>
+        <v>129</v>
+      </c>
+      <c r="CJ5" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="CK5" s="4" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="CL5" s="4" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="CM5" s="4" t="s">
         <v>247</v>
       </c>
       <c r="CN5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="CO5" s="4" t="s">
         <v>245</v>
       </c>
       <c r="CP5" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="CQ5" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="CR5" s="7" t="s">
-        <v>4</v>
+      <c r="CR5" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="CS5" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CT5" s="7" t="s">
-        <v>84</v>
+      <c r="CT5" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="CU5" s="4" t="s">
         <v>239</v>
       </c>
       <c r="CV5" s="7" t="s">
-        <v>151</v>
+        <v>48</v>
       </c>
       <c r="CW5" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="CX5" s="4" t="s">
-        <v>50</v>
+        <v>237</v>
+      </c>
+      <c r="CX5" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="CY5" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="CZ5" s="4" t="s">
-        <v>154</v>
+      <c r="CZ5" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="DA5" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="DB5" s="4" t="s">
-        <v>121</v>
+      <c r="DB5" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="DC5" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="DD5" s="14" t="s">
-        <v>92</v>
+        <v>230</v>
+      </c>
+      <c r="DD5" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="DE5" s="4" t="s">
         <v>229</v>
       </c>
       <c r="DF5" s="4" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="DG5" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="DH5" s="7" t="s">
-        <v>160</v>
+        <v>227</v>
+      </c>
+      <c r="DH5" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="DI5" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="DJ5" s="4" t="s">
-        <v>162</v>
+      <c r="DJ5" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="DK5" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="DL5" s="7" t="s">
-        <v>164</v>
+        <v>223</v>
+      </c>
+      <c r="DL5" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="DM5" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="DN5" s="7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="DO5" s="4" t="s">
         <v>219</v>
       </c>
+      <c r="DP5" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="DQ5" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="DR5" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="DS5" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="DT5" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="DU5" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
-    <row r="6" spans="1:119" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:119" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:125" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:125" x14ac:dyDescent="0.25">
       <c r="G7" s="32"/>
     </row>
   </sheetData>
@@ -3507,14 +3624,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P1048576 V6:V1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"bulk,single,inclusive"</formula1>
     </dataValidation>
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G6:G1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 DM6:DM1048576 DK6:DK1048576 DO6:DO1048576 DI6:DI1048576 DG6:DG1048576 DE6:DE1048576 DC6:DC1048576 DA6:DA1048576 CY6:CY1048576 CW6:CW1048576 CU6:CU1048576 CS6:CS1048576 CQ6:CQ1048576 CO6:CO1048576 CM6:CM1048576 CK6:CK1048576 CI6:CI1048576 CG6:CG1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 DS6:DS1048576 DQ6:DQ1048576 DU6:DU1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 DI6:DI1048576 DG6:DG1048576 DE6:DE1048576 DC6:DC1048576 DA6:DA1048576 CY6:CY1048576 CW6:CW1048576 CU6:CU1048576 CS6:CS1048576 CQ6:CQ1048576 CO6:CO1048576 CM6:CM1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3527,7 +3644,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AL6:AL1048576 AP6:AP1048576 BF6:BF1048576 AT6:AT1048576 BR6:BR1048576 BJ6:BJ1048576 BN6:BN1048576 BV6:BV1048576 AX6:AX1048576 BB6:BB1048576</xm:sqref>
+          <xm:sqref>AR6:AR1048576 AV6:AV1048576 BL6:BL1048576 AZ6:AZ1048576 BX6:BX1048576 BP6:BP1048576 BT6:BT1048576 CB6:CB1048576 BD6:BD1048576 BH6:BH1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3551,42 +3668,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3610,17 +3727,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added second extension and container blocks
</commit_message>
<xml_diff>
--- a/templates/extended_aspace_import_excel_template.xlsx
+++ b/templates/extended_aspace_import_excel_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbi\Documents\aspace\archivesspace\plugins\aspace-import-excel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbi\Documents\aspace\archivesspace_2_5_1\plugins\aspace-import-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BEC1C6-5F5D-49CB-A1C7-EAEB6136E331}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FE3DB6-A979-4F22-9AFC-EA7780587FA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="780" windowWidth="20085" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1200" windowWidth="20085" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="385">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -1100,6 +1100,90 @@
   </si>
   <si>
     <t>Dates(2)</t>
+  </si>
+  <si>
+    <t>Extent portion(2)</t>
+  </si>
+  <si>
+    <t>portion_2</t>
+  </si>
+  <si>
+    <t>number_2</t>
+  </si>
+  <si>
+    <t>Extent number(2)</t>
+  </si>
+  <si>
+    <t>extent_type_2</t>
+  </si>
+  <si>
+    <t>Extent type(2): cubic feet, cds, etc.</t>
+  </si>
+  <si>
+    <t>container_summary_2</t>
+  </si>
+  <si>
+    <t>Container Summary(2)</t>
+  </si>
+  <si>
+    <t>physical_details_2</t>
+  </si>
+  <si>
+    <t>Physical Details(2)</t>
+  </si>
+  <si>
+    <t>dimensions_2</t>
+  </si>
+  <si>
+    <t>Dimensions(2)</t>
+  </si>
+  <si>
+    <t>cont_instance_type_2</t>
+  </si>
+  <si>
+    <t>Container Instance Type(2)</t>
+  </si>
+  <si>
+    <t>type_1_2</t>
+  </si>
+  <si>
+    <t>Top Container type(2)</t>
+  </si>
+  <si>
+    <t>indicator_1_2</t>
+  </si>
+  <si>
+    <t>Top Container [indicator](2)</t>
+  </si>
+  <si>
+    <t>barcode(2)</t>
+  </si>
+  <si>
+    <t>barcode_2</t>
+  </si>
+  <si>
+    <t>type_2_2</t>
+  </si>
+  <si>
+    <t>Child type(2)</t>
+  </si>
+  <si>
+    <t>indicator_2_2</t>
+  </si>
+  <si>
+    <t>Child indicator(2)</t>
+  </si>
+  <si>
+    <t>type_3_2</t>
+  </si>
+  <si>
+    <t>Grandchild type(2)</t>
+  </si>
+  <si>
+    <t>indicator_3_2</t>
+  </si>
+  <si>
+    <t>Grandchild indicator(2)</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1301,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1299,6 +1383,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
@@ -1385,7 +1475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1566,6 +1656,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1988,7 +2081,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:APU7"/>
+  <dimension ref="A1:AQI7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2028,91 +2121,99 @@
     <col min="36" max="36" width="19.140625" style="50" customWidth="1"/>
     <col min="37" max="37" width="10.42578125" style="1" customWidth="1"/>
     <col min="38" max="38" width="11.42578125" style="50" customWidth="1"/>
-    <col min="39" max="39" width="10.42578125" style="1" customWidth="1"/>
-    <col min="40" max="41" width="9.140625" style="1"/>
-    <col min="42" max="42" width="15.28515625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="22.7109375" style="1"/>
-    <col min="44" max="44" width="15.28515625" style="1" customWidth="1"/>
-    <col min="45" max="45" width="13" style="1" customWidth="1"/>
-    <col min="46" max="46" width="15.42578125" style="1" customWidth="1"/>
-    <col min="47" max="47" width="22.7109375" style="1"/>
-    <col min="48" max="48" width="15.28515625" style="1" customWidth="1"/>
-    <col min="49" max="49" width="9.140625" style="1"/>
-    <col min="50" max="50" width="15.140625" style="1" customWidth="1"/>
-    <col min="51" max="51" width="20.140625" style="1" customWidth="1"/>
-    <col min="52" max="52" width="15.28515625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="12.85546875" style="1" customWidth="1"/>
-    <col min="54" max="54" width="15.140625" style="1" customWidth="1"/>
-    <col min="55" max="55" width="20.140625" style="1" customWidth="1"/>
+    <col min="39" max="45" width="26.85546875" style="1" customWidth="1"/>
+    <col min="46" max="46" width="9.140625" style="1"/>
+    <col min="47" max="47" width="9.140625" style="50"/>
+    <col min="48" max="48" width="10.42578125" style="1" customWidth="1"/>
+    <col min="49" max="49" width="19" style="50" customWidth="1"/>
+    <col min="50" max="50" width="19.140625" style="50" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" style="1" customWidth="1"/>
+    <col min="52" max="52" width="11.42578125" style="50" customWidth="1"/>
+    <col min="53" max="53" width="10.42578125" style="1" customWidth="1"/>
+    <col min="54" max="55" width="9.140625" style="1"/>
     <col min="56" max="56" width="15.28515625" style="1" customWidth="1"/>
-    <col min="57" max="57" width="12.85546875" style="1" customWidth="1"/>
-    <col min="58" max="58" width="15.140625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="20.140625" style="1" customWidth="1"/>
-    <col min="60" max="60" width="15.28515625" style="1" customWidth="1"/>
-    <col min="61" max="61" width="12.85546875" style="1" customWidth="1"/>
-    <col min="62" max="62" width="9.140625" style="1"/>
-    <col min="63" max="63" width="11.42578125" style="1" customWidth="1"/>
-    <col min="64" max="64" width="15.28515625" style="1" customWidth="1"/>
-    <col min="65" max="66" width="9.140625" style="1"/>
-    <col min="67" max="67" width="11.42578125" style="1" customWidth="1"/>
-    <col min="68" max="68" width="15.28515625" style="1" customWidth="1"/>
-    <col min="69" max="71" width="9.140625" style="1"/>
-    <col min="72" max="72" width="15.28515625" style="1" customWidth="1"/>
-    <col min="73" max="75" width="9.140625" style="1"/>
-    <col min="76" max="76" width="15.28515625" style="1" customWidth="1"/>
-    <col min="77" max="79" width="9.140625" style="1"/>
-    <col min="80" max="80" width="15.28515625" style="1" customWidth="1"/>
-    <col min="81" max="81" width="9.140625" style="1"/>
-    <col min="82" max="82" width="11.5703125" style="1" customWidth="1"/>
-    <col min="83" max="83" width="12.28515625" style="1" customWidth="1"/>
-    <col min="84" max="86" width="13.5703125" style="1" customWidth="1"/>
-    <col min="87" max="88" width="10.85546875" style="1" customWidth="1"/>
-    <col min="89" max="89" width="15.42578125" style="1" customWidth="1"/>
-    <col min="90" max="90" width="9.28515625" style="1"/>
-    <col min="91" max="91" width="17.7109375" style="1" customWidth="1"/>
-    <col min="92" max="92" width="17" style="1" customWidth="1"/>
-    <col min="93" max="93" width="17.7109375" style="1" customWidth="1"/>
-    <col min="94" max="94" width="12.28515625" style="1" customWidth="1"/>
-    <col min="95" max="95" width="17.7109375" style="1" customWidth="1"/>
-    <col min="96" max="96" width="11.7109375" style="1" customWidth="1"/>
-    <col min="97" max="97" width="17.7109375" style="1" customWidth="1"/>
-    <col min="98" max="98" width="16" style="1" customWidth="1"/>
-    <col min="99" max="99" width="17.7109375" style="1" customWidth="1"/>
-    <col min="100" max="100" width="9.140625" style="1"/>
-    <col min="101" max="101" width="17.7109375" style="1" customWidth="1"/>
-    <col min="102" max="102" width="12" customWidth="1"/>
-    <col min="103" max="103" width="17.7109375" style="1" customWidth="1"/>
-    <col min="104" max="104" width="11.85546875" style="1" customWidth="1"/>
+    <col min="57" max="57" width="22.7109375" style="1"/>
+    <col min="58" max="58" width="15.28515625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="13" style="1" customWidth="1"/>
+    <col min="60" max="60" width="15.42578125" style="1" customWidth="1"/>
+    <col min="61" max="61" width="22.7109375" style="1"/>
+    <col min="62" max="62" width="15.28515625" style="1" customWidth="1"/>
+    <col min="63" max="63" width="9.140625" style="1"/>
+    <col min="64" max="64" width="15.140625" style="1" customWidth="1"/>
+    <col min="65" max="65" width="20.140625" style="1" customWidth="1"/>
+    <col min="66" max="66" width="15.28515625" style="1" customWidth="1"/>
+    <col min="67" max="67" width="12.85546875" style="1" customWidth="1"/>
+    <col min="68" max="68" width="15.140625" style="1" customWidth="1"/>
+    <col min="69" max="69" width="20.140625" style="1" customWidth="1"/>
+    <col min="70" max="70" width="15.28515625" style="1" customWidth="1"/>
+    <col min="71" max="71" width="12.85546875" style="1" customWidth="1"/>
+    <col min="72" max="72" width="15.140625" style="1" customWidth="1"/>
+    <col min="73" max="73" width="20.140625" style="1" customWidth="1"/>
+    <col min="74" max="74" width="15.28515625" style="1" customWidth="1"/>
+    <col min="75" max="75" width="12.85546875" style="1" customWidth="1"/>
+    <col min="76" max="76" width="9.140625" style="1"/>
+    <col min="77" max="77" width="11.42578125" style="1" customWidth="1"/>
+    <col min="78" max="78" width="15.28515625" style="1" customWidth="1"/>
+    <col min="79" max="80" width="9.140625" style="1"/>
+    <col min="81" max="81" width="11.42578125" style="1" customWidth="1"/>
+    <col min="82" max="82" width="15.28515625" style="1" customWidth="1"/>
+    <col min="83" max="85" width="9.140625" style="1"/>
+    <col min="86" max="86" width="15.28515625" style="1" customWidth="1"/>
+    <col min="87" max="89" width="9.140625" style="1"/>
+    <col min="90" max="90" width="15.28515625" style="1" customWidth="1"/>
+    <col min="91" max="93" width="9.140625" style="1"/>
+    <col min="94" max="94" width="15.28515625" style="1" customWidth="1"/>
+    <col min="95" max="95" width="9.140625" style="1"/>
+    <col min="96" max="96" width="11.5703125" style="1" customWidth="1"/>
+    <col min="97" max="97" width="12.28515625" style="1" customWidth="1"/>
+    <col min="98" max="100" width="13.5703125" style="1" customWidth="1"/>
+    <col min="101" max="102" width="10.85546875" style="1" customWidth="1"/>
+    <col min="103" max="103" width="15.42578125" style="1" customWidth="1"/>
+    <col min="104" max="104" width="9.28515625" style="1"/>
     <col min="105" max="105" width="17.7109375" style="1" customWidth="1"/>
-    <col min="106" max="106" width="11.85546875" style="1" customWidth="1"/>
+    <col min="106" max="106" width="17" style="1" customWidth="1"/>
     <col min="107" max="107" width="17.7109375" style="1" customWidth="1"/>
-    <col min="108" max="108" width="11.85546875" style="1" customWidth="1"/>
+    <col min="108" max="108" width="12.28515625" style="1" customWidth="1"/>
     <col min="109" max="109" width="17.7109375" style="1" customWidth="1"/>
-    <col min="110" max="110" width="11.85546875" style="1" customWidth="1"/>
+    <col min="110" max="110" width="11.7109375" style="1" customWidth="1"/>
     <col min="111" max="111" width="17.7109375" style="1" customWidth="1"/>
-    <col min="112" max="112" width="11.85546875" style="1" customWidth="1"/>
+    <col min="112" max="112" width="16" style="1" customWidth="1"/>
     <col min="113" max="113" width="17.7109375" style="1" customWidth="1"/>
-    <col min="114" max="114" width="14.85546875" style="1" customWidth="1"/>
+    <col min="114" max="114" width="9.140625" style="1"/>
     <col min="115" max="115" width="17.7109375" style="1" customWidth="1"/>
-    <col min="116" max="116" width="12.28515625" style="1" customWidth="1"/>
+    <col min="116" max="116" width="12" customWidth="1"/>
     <col min="117" max="117" width="17.7109375" style="1" customWidth="1"/>
-    <col min="118" max="118" width="9.140625" style="1"/>
+    <col min="118" max="118" width="11.85546875" style="1" customWidth="1"/>
     <col min="119" max="119" width="17.7109375" style="1" customWidth="1"/>
-    <col min="120" max="120" width="9.140625" style="1"/>
+    <col min="120" max="120" width="11.85546875" style="1" customWidth="1"/>
     <col min="121" max="121" width="17.7109375" style="1" customWidth="1"/>
-    <col min="122" max="122" width="18.42578125" style="1" customWidth="1"/>
+    <col min="122" max="122" width="11.85546875" style="1" customWidth="1"/>
     <col min="123" max="123" width="17.7109375" style="1" customWidth="1"/>
-    <col min="124" max="124" width="10.140625" style="1" customWidth="1"/>
+    <col min="124" max="124" width="11.85546875" style="1" customWidth="1"/>
     <col min="125" max="125" width="17.7109375" style="1" customWidth="1"/>
-    <col min="126" max="1113" width="9.28515625" style="1"/>
+    <col min="126" max="126" width="11.85546875" style="1" customWidth="1"/>
+    <col min="127" max="127" width="17.7109375" style="1" customWidth="1"/>
+    <col min="128" max="128" width="14.85546875" style="1" customWidth="1"/>
+    <col min="129" max="129" width="17.7109375" style="1" customWidth="1"/>
+    <col min="130" max="130" width="12.28515625" style="1" customWidth="1"/>
+    <col min="131" max="131" width="17.7109375" style="1" customWidth="1"/>
+    <col min="132" max="132" width="9.140625" style="1"/>
+    <col min="133" max="133" width="17.7109375" style="1" customWidth="1"/>
+    <col min="134" max="134" width="9.140625" style="1"/>
+    <col min="135" max="135" width="17.7109375" style="1" customWidth="1"/>
+    <col min="136" max="136" width="18.42578125" style="1" customWidth="1"/>
+    <col min="137" max="137" width="17.7109375" style="1" customWidth="1"/>
+    <col min="138" max="138" width="10.140625" style="1" customWidth="1"/>
+    <col min="139" max="139" width="17.7109375" style="1" customWidth="1"/>
+    <col min="140" max="1127" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:125" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:139" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:125" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:139" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -2227,56 +2328,56 @@
       <c r="AL2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AM2" s="22" t="s">
+      <c r="AM2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AU2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AY2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AZ2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="BA2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="AN2" s="22" t="s">
+      <c r="BB2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="23" t="s">
+      <c r="BC2" s="23" t="s">
         <v>41</v>
-      </c>
-      <c r="AP2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="BC2" s="19" t="s">
-        <v>1</v>
       </c>
       <c r="BD2" s="48" t="s">
         <v>1</v>
@@ -2284,143 +2385,143 @@
       <c r="BE2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BF2" s="19" t="s">
+      <c r="BF2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BG2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BH2" s="48" t="s">
+      <c r="BH2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BI2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BJ2" s="19" t="s">
+      <c r="BJ2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BK2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BL2" s="48" t="s">
+      <c r="BL2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BM2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BN2" s="19" t="s">
+      <c r="BN2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BO2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BP2" s="48" t="s">
+      <c r="BP2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BQ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BR2" s="19" t="s">
+      <c r="BR2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BS2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BT2" s="48" t="s">
+      <c r="BT2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BU2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BV2" s="19" t="s">
+      <c r="BV2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BW2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BX2" s="48" t="s">
+      <c r="BX2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BY2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BZ2" s="19" t="s">
+      <c r="BZ2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CA2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CB2" s="48" t="s">
+      <c r="CB2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="CC2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CD2" s="19" t="s">
+      <c r="CD2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="CE2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CG2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CK2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CL2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="CM2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CN2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CO2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CP2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="CQ2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="CR2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CE2" s="19" t="s">
+      <c r="CS2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CF2" s="19" t="s">
+      <c r="CT2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CG2" s="19" t="s">
+      <c r="CU2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CH2" s="19" t="s">
+      <c r="CV2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CI2" s="19" t="s">
+      <c r="CW2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CJ2" s="19" t="s">
+      <c r="CX2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CK2" s="19" t="s">
+      <c r="CY2" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="CL2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CM2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CN2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CO2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CP2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CQ2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CR2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CS2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CT2" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="CU2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CV2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CW2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CX2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="CY2" s="29" t="s">
-        <v>65</v>
       </c>
       <c r="CZ2" s="29" t="s">
         <v>65</v>
@@ -2446,13 +2547,13 @@
       <c r="DG2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="DH2" s="29" t="s">
+      <c r="DH2" s="28" t="s">
         <v>65</v>
       </c>
       <c r="DI2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="DJ2" s="30" t="s">
+      <c r="DJ2" s="29" t="s">
         <v>65</v>
       </c>
       <c r="DK2" s="29" t="s">
@@ -2488,8 +2589,50 @@
       <c r="DU2" s="29" t="s">
         <v>65</v>
       </c>
+      <c r="DV2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DW2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DX2" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="DY2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DZ2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EA2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EB2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EC2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="ED2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EE2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EF2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EG2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EH2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EI2" s="29" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="3" spans="1:125" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:139" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>68</v>
       </c>
@@ -2602,269 +2745,311 @@
       <c r="AL3" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="AM3" s="24" t="s">
+      <c r="AM3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS3" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="AT3" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="AU3" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW3" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="AX3" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ3" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AN3" s="25" t="s">
+      <c r="BB3" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="AO3" s="24" t="s">
+      <c r="BC3" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="AP3" s="27" t="s">
+      <c r="BD3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="AQ3" s="27" t="s">
+      <c r="BE3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="AR3" s="27" t="s">
+      <c r="BF3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="AS3" s="27" t="s">
+      <c r="BG3" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="AT3" s="27" t="s">
+      <c r="BH3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="AU3" s="27" t="s">
+      <c r="BI3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="AV3" s="27" t="s">
+      <c r="BJ3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="AW3" s="27" t="s">
+      <c r="BK3" s="27" t="s">
         <v>295</v>
       </c>
-      <c r="AX3" s="27" t="s">
+      <c r="BL3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="AY3" s="27" t="s">
+      <c r="BM3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="AZ3" s="27" t="s">
+      <c r="BN3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BA3" s="27" t="s">
+      <c r="BO3" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="BB3" s="27" t="s">
+      <c r="BP3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BC3" s="27" t="s">
+      <c r="BQ3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BD3" s="27" t="s">
+      <c r="BR3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BE3" s="27" t="s">
+      <c r="BS3" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="BF3" s="27" t="s">
+      <c r="BT3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BG3" s="27" t="s">
+      <c r="BU3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BH3" s="27" t="s">
+      <c r="BV3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BI3" s="27" t="s">
+      <c r="BW3" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="BJ3" s="27" t="s">
+      <c r="BX3" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="BK3" s="27" t="s">
+      <c r="BY3" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="BL3" s="27" t="s">
+      <c r="BZ3" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="BM3" s="27" t="s">
+      <c r="CA3" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="BN3" s="27" t="s">
+      <c r="CB3" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="BO3" s="27" t="s">
+      <c r="CC3" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="BP3" s="27" t="s">
+      <c r="CD3" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="BQ3" s="27" t="s">
+      <c r="CE3" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="BR3" s="27" t="s">
+      <c r="CF3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="BS3" s="27" t="s">
+      <c r="CG3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="BT3" s="27" t="s">
+      <c r="CH3" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="BU3" s="27" t="s">
+      <c r="CI3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="BV3" s="27" t="s">
+      <c r="CJ3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="BW3" s="27" t="s">
+      <c r="CK3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="BX3" s="27" t="s">
+      <c r="CL3" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="BY3" s="27" t="s">
+      <c r="CM3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="BZ3" s="27" t="s">
+      <c r="CN3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="CA3" s="27" t="s">
+      <c r="CO3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="CB3" s="27" t="s">
+      <c r="CP3" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="CC3" s="27" t="s">
+      <c r="CQ3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="CD3" s="27" t="s">
+      <c r="CR3" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="CE3" s="27" t="s">
+      <c r="CS3" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="CF3" s="27" t="s">
+      <c r="CT3" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="CG3" s="27" t="s">
+      <c r="CU3" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="CH3" s="27" t="s">
+      <c r="CV3" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="CI3" s="27" t="s">
+      <c r="CW3" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="CJ3" s="27" t="s">
+      <c r="CX3" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="CK3" s="27" t="s">
+      <c r="CY3" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="CL3" s="26" t="s">
+      <c r="CZ3" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="CM3" s="59" t="s">
+      <c r="DA3" s="59" t="s">
         <v>246</v>
       </c>
-      <c r="CN3" s="26" t="s">
+      <c r="DB3" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="CO3" s="59" t="s">
+      <c r="DC3" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="CP3" s="26" t="s">
+      <c r="DD3" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="CQ3" s="59" t="s">
+      <c r="DE3" s="59" t="s">
         <v>242</v>
       </c>
-      <c r="CR3" s="26" t="s">
+      <c r="DF3" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="CS3" s="59" t="s">
+      <c r="DG3" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="CT3" s="26" t="s">
+      <c r="DH3" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="CU3" s="59" t="s">
+      <c r="DI3" s="59" t="s">
         <v>238</v>
       </c>
-      <c r="CV3" s="26" t="s">
+      <c r="DJ3" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="CW3" s="59" t="s">
+      <c r="DK3" s="59" t="s">
         <v>236</v>
       </c>
-      <c r="CX3" s="26" t="s">
+      <c r="DL3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="CY3" s="59" t="s">
+      <c r="DM3" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="CZ3" s="26" t="s">
+      <c r="DN3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DA3" s="59" t="s">
+      <c r="DO3" s="59" t="s">
         <v>232</v>
       </c>
-      <c r="DB3" s="26" t="s">
+      <c r="DP3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="DC3" s="59" t="s">
+      <c r="DQ3" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="DD3" s="26" t="s">
+      <c r="DR3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DE3" s="59" t="s">
+      <c r="DS3" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="DF3" s="26" t="s">
+      <c r="DT3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="DG3" s="59" t="s">
+      <c r="DU3" s="59" t="s">
         <v>226</v>
       </c>
-      <c r="DH3" s="26" t="s">
+      <c r="DV3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="DI3" s="59" t="s">
+      <c r="DW3" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="DJ3" s="26" t="s">
+      <c r="DX3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="DK3" s="59" t="s">
+      <c r="DY3" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="DL3" s="26" t="s">
+      <c r="DZ3" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="DM3" s="59" t="s">
+      <c r="EA3" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="DN3" s="26" t="s">
+      <c r="EB3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="DO3" s="59" t="s">
+      <c r="EC3" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="DP3" s="26" t="s">
+      <c r="ED3" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="DQ3" s="59" t="s">
+      <c r="EE3" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="DR3" s="26" t="s">
+      <c r="EF3" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="DS3" s="59" t="s">
+      <c r="EG3" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="DT3" s="26" t="s">
+      <c r="EH3" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="DU3" s="59" t="s">
+      <c r="EI3" s="59" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:125" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:139" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
@@ -2980,268 +3165,310 @@
         <v>34</v>
       </c>
       <c r="AM4" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="AN4" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="AO4" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="AP4" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="AQ4" s="38" t="s">
+        <v>365</v>
+      </c>
+      <c r="AR4" s="61" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS4" s="38" t="s">
+        <v>369</v>
+      </c>
+      <c r="AT4" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="AU4" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="AV4" s="38" t="s">
+        <v>376</v>
+      </c>
+      <c r="AW4" s="40" t="s">
+        <v>377</v>
+      </c>
+      <c r="AX4" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="AY4" s="38" t="s">
+        <v>381</v>
+      </c>
+      <c r="AZ4" s="40" t="s">
+        <v>383</v>
+      </c>
+      <c r="BA4" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="AN4" s="38" t="s">
+      <c r="BB4" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="AO4" s="38" t="s">
+      <c r="BC4" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="AP4" s="38" t="s">
+      <c r="BD4" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="AQ4" s="38" t="s">
+      <c r="BE4" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="AR4" s="38" t="s">
+      <c r="BF4" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="AS4" s="38" t="s">
+      <c r="BG4" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="AT4" s="38" t="s">
+      <c r="BH4" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="AU4" s="38" t="s">
+      <c r="BI4" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="AV4" s="38" t="s">
+      <c r="BJ4" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="38" t="s">
+      <c r="BK4" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="AX4" s="38" t="s">
+      <c r="BL4" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="AY4" s="38" t="s">
+      <c r="BM4" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AZ4" s="38" t="s">
+      <c r="BN4" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="BA4" s="38" t="s">
+      <c r="BO4" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="BB4" s="38" t="s">
+      <c r="BP4" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="BC4" s="38" t="s">
+      <c r="BQ4" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="BD4" s="38" t="s">
+      <c r="BR4" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="BE4" s="38" t="s">
+      <c r="BS4" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="BF4" s="38" t="s">
+      <c r="BT4" s="38" t="s">
         <v>328</v>
       </c>
-      <c r="BG4" s="38" t="s">
+      <c r="BU4" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="BH4" s="38" t="s">
+      <c r="BV4" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="BI4" s="38" t="s">
+      <c r="BW4" s="38" t="s">
         <v>334</v>
       </c>
-      <c r="BJ4" s="38" t="s">
+      <c r="BX4" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="BK4" s="38" t="s">
+      <c r="BY4" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="BL4" s="38" t="s">
+      <c r="BZ4" s="38" t="s">
         <v>287</v>
       </c>
-      <c r="BM4" s="38" t="s">
+      <c r="CA4" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="BN4" s="38" t="s">
+      <c r="CB4" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="BO4" s="38" t="s">
+      <c r="CC4" s="38" t="s">
         <v>303</v>
       </c>
-      <c r="BP4" s="38" t="s">
+      <c r="CD4" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="BQ4" s="38" t="s">
+      <c r="CE4" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="BR4" s="38" t="s">
+      <c r="CF4" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="BS4" s="38" t="s">
+      <c r="CG4" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="BT4" s="38" t="s">
+      <c r="CH4" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="BU4" s="38" t="s">
+      <c r="CI4" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="BV4" s="38" t="s">
+      <c r="CJ4" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="BW4" s="38" t="s">
+      <c r="CK4" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="BX4" s="38" t="s">
+      <c r="CL4" s="38" t="s">
         <v>292</v>
       </c>
-      <c r="BY4" s="38" t="s">
+      <c r="CM4" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="BZ4" s="38" t="s">
+      <c r="CN4" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="CA4" s="38" t="s">
+      <c r="CO4" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="CB4" s="38" t="s">
+      <c r="CP4" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="CC4" s="38" t="s">
+      <c r="CQ4" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="CD4" s="38" t="s">
+      <c r="CR4" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="CE4" s="38" t="s">
+      <c r="CS4" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="CF4" s="38" t="s">
+      <c r="CT4" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="CG4" s="38" t="s">
+      <c r="CU4" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="CH4" s="38" t="s">
+      <c r="CV4" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="CI4" s="38" t="s">
+      <c r="CW4" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="CJ4" s="38" t="s">
+      <c r="CX4" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="CK4" s="38" t="s">
+      <c r="CY4" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="CL4" s="38" t="s">
+      <c r="CZ4" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="CM4" s="38" t="s">
+      <c r="DA4" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="CN4" s="38" t="s">
+      <c r="DB4" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="CO4" s="38" t="s">
+      <c r="DC4" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="CP4" s="41" t="s">
+      <c r="DD4" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="CQ4" s="38" t="s">
+      <c r="DE4" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="CR4" s="38" t="s">
+      <c r="DF4" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="CS4" s="38" t="s">
+      <c r="DG4" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="CT4" s="38" t="s">
+      <c r="DH4" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="CU4" s="38" t="s">
+      <c r="DI4" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="CV4" s="41" t="s">
+      <c r="DJ4" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="CW4" s="38" t="s">
+      <c r="DK4" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="CX4" s="41" t="s">
+      <c r="DL4" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="CY4" s="38" t="s">
+      <c r="DM4" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="CZ4" s="41" t="s">
+      <c r="DN4" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="DA4" s="38" t="s">
+      <c r="DO4" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="DB4" s="41" t="s">
+      <c r="DP4" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="DC4" s="38" t="s">
+      <c r="DQ4" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="DD4" s="38" t="s">
+      <c r="DR4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="DE4" s="38" t="s">
+      <c r="DS4" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="DF4" s="38" t="s">
+      <c r="DT4" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="DG4" s="38" t="s">
+      <c r="DU4" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="DH4" s="38" t="s">
+      <c r="DV4" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="DI4" s="38" t="s">
+      <c r="DW4" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="DJ4" s="41" t="s">
+      <c r="DX4" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="DK4" s="38" t="s">
+      <c r="DY4" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="DL4" s="38" t="s">
+      <c r="DZ4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="DM4" s="38" t="s">
+      <c r="EA4" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="DN4" s="41" t="s">
+      <c r="EB4" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="DO4" s="38" t="s">
+      <c r="EC4" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="DP4" s="38" t="s">
+      <c r="ED4" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="DQ4" s="38" t="s">
+      <c r="EE4" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="DR4" s="41" t="s">
+      <c r="EF4" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="DS4" s="41" t="s">
+      <c r="EG4" s="41" t="s">
         <v>264</v>
       </c>
-      <c r="DT4" s="41" t="s">
+      <c r="EH4" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="DU4" s="38" t="s">
+      <c r="EI4" s="38" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:125" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:139" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>67</v>
       </c>
@@ -3357,269 +3584,311 @@
         <v>91</v>
       </c>
       <c r="AM5" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="AN5" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="AO5" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="AU5" s="53" t="s">
+        <v>374</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="AW5" s="53" t="s">
+        <v>378</v>
+      </c>
+      <c r="AX5" s="53" t="s">
+        <v>380</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="AZ5" s="53" t="s">
+        <v>384</v>
+      </c>
+      <c r="BA5" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AN5" s="4" t="s">
+      <c r="BB5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="BC5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="BD5" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="BE5" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="BF5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="AS5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="AT5" s="4" t="s">
+      <c r="BH5" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="AU5" s="4" t="s">
+      <c r="BI5" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="AV5" s="4" t="s">
+      <c r="BJ5" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="AW5" s="4" t="s">
+      <c r="BK5" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="AX5" s="4" t="s">
+      <c r="BL5" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="AY5" s="4" t="s">
+      <c r="BM5" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="AZ5" s="4" t="s">
+      <c r="BN5" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="BA5" s="4" t="s">
+      <c r="BO5" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="BB5" s="4" t="s">
+      <c r="BP5" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="BC5" s="4" t="s">
+      <c r="BQ5" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="BD5" s="4" t="s">
+      <c r="BR5" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="BE5" s="4" t="s">
+      <c r="BS5" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="BF5" s="4" t="s">
+      <c r="BT5" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="BG5" s="4" t="s">
+      <c r="BU5" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="BH5" s="4" t="s">
+      <c r="BV5" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="BI5" s="4" t="s">
+      <c r="BW5" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="BJ5" s="4" t="s">
+      <c r="BX5" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="BK5" s="4" t="s">
+      <c r="BY5" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="BL5" s="4" t="s">
+      <c r="BZ5" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="BM5" s="4" t="s">
+      <c r="CA5" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="BN5" s="4" t="s">
+      <c r="CB5" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="BO5" s="4" t="s">
+      <c r="CC5" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="BP5" s="4" t="s">
+      <c r="CD5" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="BQ5" s="4" t="s">
+      <c r="CE5" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="BR5" s="4" t="s">
+      <c r="CF5" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="BS5" s="4" t="s">
+      <c r="CG5" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="BT5" s="4" t="s">
+      <c r="CH5" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="BU5" s="4" t="s">
+      <c r="CI5" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="BV5" s="4" t="s">
+      <c r="CJ5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="BW5" s="4" t="s">
+      <c r="CK5" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="BX5" s="4" t="s">
+      <c r="CL5" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="BY5" s="4" t="s">
+      <c r="CM5" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="BZ5" s="4" t="s">
+      <c r="CN5" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="CA5" s="4" t="s">
+      <c r="CO5" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="CB5" s="4" t="s">
+      <c r="CP5" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="CC5" s="4" t="s">
+      <c r="CQ5" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="CD5" s="4" t="s">
+      <c r="CR5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="CE5" s="4" t="s">
+      <c r="CS5" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="CF5" s="4" t="s">
+      <c r="CT5" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="CG5" s="4" t="s">
+      <c r="CU5" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="CH5" s="4" t="s">
+      <c r="CV5" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="CI5" s="4" t="s">
+      <c r="CW5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="CJ5" s="4" t="s">
+      <c r="CX5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="CK5" s="4" t="s">
+      <c r="CY5" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="CL5" s="4" t="s">
+      <c r="CZ5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="CM5" s="4" t="s">
+      <c r="DA5" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="CN5" s="4" t="s">
+      <c r="DB5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="CO5" s="4" t="s">
+      <c r="DC5" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="CP5" s="7" t="s">
+      <c r="DD5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="CQ5" s="4" t="s">
+      <c r="DE5" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="CR5" s="4" t="s">
+      <c r="DF5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="CS5" s="4" t="s">
+      <c r="DG5" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CT5" s="4" t="s">
+      <c r="DH5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="CU5" s="4" t="s">
+      <c r="DI5" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="CV5" s="7" t="s">
+      <c r="DJ5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="CW5" s="4" t="s">
+      <c r="DK5" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="CX5" s="7" t="s">
+      <c r="DL5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="CY5" s="4" t="s">
+      <c r="DM5" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="CZ5" s="7" t="s">
+      <c r="DN5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="DA5" s="4" t="s">
+      <c r="DO5" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="DB5" s="7" t="s">
+      <c r="DP5" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="DC5" s="4" t="s">
+      <c r="DQ5" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="DD5" s="4" t="s">
+      <c r="DR5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="DE5" s="4" t="s">
+      <c r="DS5" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="DF5" s="4" t="s">
+      <c r="DT5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="DG5" s="4" t="s">
+      <c r="DU5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="DH5" s="4" t="s">
+      <c r="DV5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="DI5" s="4" t="s">
+      <c r="DW5" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="DJ5" s="14" t="s">
+      <c r="DX5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="DK5" s="4" t="s">
+      <c r="DY5" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="DL5" s="4" t="s">
+      <c r="DZ5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="DM5" s="4" t="s">
+      <c r="EA5" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="DN5" s="7" t="s">
+      <c r="EB5" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="DO5" s="4" t="s">
+      <c r="EC5" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="DP5" s="4" t="s">
+      <c r="ED5" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="DQ5" s="4" t="s">
+      <c r="EE5" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="DR5" s="7" t="s">
+      <c r="EF5" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="DS5" s="4" t="s">
+      <c r="EG5" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="DT5" s="7" t="s">
+      <c r="EH5" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="DU5" s="4" t="s">
+      <c r="EI5" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:125" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:139" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:139" x14ac:dyDescent="0.25">
       <c r="G7" s="32"/>
     </row>
   </sheetData>
@@ -3637,7 +3906,7 @@
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 DS6:DS1048576 DQ6:DQ1048576 DU6:DU1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 DI6:DI1048576 DG6:DG1048576 DE6:DE1048576 DC6:DC1048576 DA6:DA1048576 CY6:CY1048576 CW6:CW1048576 CU6:CU1048576 CS6:CS1048576 CQ6:CQ1048576 CO6:CO1048576 CM6:CM1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 EG6:EG1048576 EE6:EE1048576 EI6:EI1048576 EC6:EC1048576 EA6:EA1048576 DY6:DY1048576 DW6:DW1048576 DU6:DU1048576 DS6:DS1048576 DQ6:DQ1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 DI6:DI1048576 DG6:DG1048576 DE6:DE1048576 DC6:DC1048576 DA6:DA1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3650,7 +3919,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AR6:AR1048576 AV6:AV1048576 BL6:BL1048576 AZ6:AZ1048576 BX6:BX1048576 BP6:BP1048576 BT6:BT1048576 CB6:CB1048576 BD6:BD1048576 BH6:BH1048576</xm:sqref>
+          <xm:sqref>BF6:BF1048576 BJ6:BJ1048576 BZ6:BZ1048576 BN6:BN1048576 CL6:CL1048576 CD6:CD1048576 CH6:CH1048576 CP6:CP1048576 BR6:BR1048576 BV6:BV1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
added second extent block
</commit_message>
<xml_diff>
--- a/templates/extended_aspace_import_excel_template.xlsx
+++ b/templates/extended_aspace_import_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbi\Documents\aspace\archivesspace_2_5_1\plugins\aspace-import-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FE3DB6-A979-4F22-9AFC-EA7780587FA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C869A4D-87B6-4029-8803-46342D4B3942}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="1200" windowWidth="20085" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="389">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -1184,6 +1184,18 @@
   </si>
   <si>
     <t>Grandchild indicator(2)</t>
+  </si>
+  <si>
+    <t>Extent(2) portion</t>
+  </si>
+  <si>
+    <t>Extent(2) number</t>
+  </si>
+  <si>
+    <t>Extent(2) type: cubic feet, cds, etc.</t>
+  </si>
+  <si>
+    <t>Container Summary (2)</t>
   </si>
 </sst>
 </file>
@@ -2081,11 +2093,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQI7"/>
+  <dimension ref="A1:AQO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,107 +2125,107 @@
     <col min="21" max="21" width="10.5703125" style="50" customWidth="1"/>
     <col min="22" max="22" width="23.85546875" style="1" customWidth="1"/>
     <col min="23" max="23" width="15.140625" style="50" customWidth="1"/>
-    <col min="24" max="31" width="26.85546875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="23" style="1"/>
-    <col min="33" max="33" width="23" style="50"/>
-    <col min="34" max="34" width="10.42578125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="19" style="50" customWidth="1"/>
-    <col min="36" max="36" width="19.140625" style="50" customWidth="1"/>
-    <col min="37" max="37" width="10.42578125" style="1" customWidth="1"/>
-    <col min="38" max="38" width="11.42578125" style="50" customWidth="1"/>
-    <col min="39" max="45" width="26.85546875" style="1" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="1"/>
-    <col min="47" max="47" width="9.140625" style="50"/>
-    <col min="48" max="48" width="10.42578125" style="1" customWidth="1"/>
-    <col min="49" max="49" width="19" style="50" customWidth="1"/>
-    <col min="50" max="50" width="19.140625" style="50" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" style="1" customWidth="1"/>
-    <col min="52" max="52" width="11.42578125" style="50" customWidth="1"/>
-    <col min="53" max="53" width="10.42578125" style="1" customWidth="1"/>
-    <col min="54" max="55" width="9.140625" style="1"/>
-    <col min="56" max="56" width="15.28515625" style="1" customWidth="1"/>
-    <col min="57" max="57" width="22.7109375" style="1"/>
-    <col min="58" max="58" width="15.28515625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="13" style="1" customWidth="1"/>
-    <col min="60" max="60" width="15.42578125" style="1" customWidth="1"/>
-    <col min="61" max="61" width="22.7109375" style="1"/>
+    <col min="24" max="37" width="26.85546875" style="1" customWidth="1"/>
+    <col min="38" max="38" width="23" style="1"/>
+    <col min="39" max="39" width="23" style="50"/>
+    <col min="40" max="40" width="10.42578125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="19" style="50" customWidth="1"/>
+    <col min="42" max="42" width="19.140625" style="50" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="11.42578125" style="50" customWidth="1"/>
+    <col min="45" max="51" width="26.85546875" style="1" customWidth="1"/>
+    <col min="52" max="52" width="9.140625" style="1"/>
+    <col min="53" max="53" width="9.140625" style="50"/>
+    <col min="54" max="54" width="10.42578125" style="1" customWidth="1"/>
+    <col min="55" max="55" width="19" style="50" customWidth="1"/>
+    <col min="56" max="56" width="19.140625" style="50" customWidth="1"/>
+    <col min="57" max="57" width="10.42578125" style="1" customWidth="1"/>
+    <col min="58" max="58" width="11.42578125" style="50" customWidth="1"/>
+    <col min="59" max="59" width="10.42578125" style="1" customWidth="1"/>
+    <col min="60" max="61" width="9.140625" style="1"/>
     <col min="62" max="62" width="15.28515625" style="1" customWidth="1"/>
-    <col min="63" max="63" width="9.140625" style="1"/>
-    <col min="64" max="64" width="15.140625" style="1" customWidth="1"/>
-    <col min="65" max="65" width="20.140625" style="1" customWidth="1"/>
-    <col min="66" max="66" width="15.28515625" style="1" customWidth="1"/>
-    <col min="67" max="67" width="12.85546875" style="1" customWidth="1"/>
-    <col min="68" max="68" width="15.140625" style="1" customWidth="1"/>
-    <col min="69" max="69" width="20.140625" style="1" customWidth="1"/>
-    <col min="70" max="70" width="15.28515625" style="1" customWidth="1"/>
-    <col min="71" max="71" width="12.85546875" style="1" customWidth="1"/>
-    <col min="72" max="72" width="15.140625" style="1" customWidth="1"/>
-    <col min="73" max="73" width="20.140625" style="1" customWidth="1"/>
-    <col min="74" max="74" width="15.28515625" style="1" customWidth="1"/>
-    <col min="75" max="75" width="12.85546875" style="1" customWidth="1"/>
-    <col min="76" max="76" width="9.140625" style="1"/>
-    <col min="77" max="77" width="11.42578125" style="1" customWidth="1"/>
-    <col min="78" max="78" width="15.28515625" style="1" customWidth="1"/>
-    <col min="79" max="80" width="9.140625" style="1"/>
-    <col min="81" max="81" width="11.42578125" style="1" customWidth="1"/>
-    <col min="82" max="82" width="15.28515625" style="1" customWidth="1"/>
-    <col min="83" max="85" width="9.140625" style="1"/>
-    <col min="86" max="86" width="15.28515625" style="1" customWidth="1"/>
-    <col min="87" max="89" width="9.140625" style="1"/>
-    <col min="90" max="90" width="15.28515625" style="1" customWidth="1"/>
-    <col min="91" max="93" width="9.140625" style="1"/>
-    <col min="94" max="94" width="15.28515625" style="1" customWidth="1"/>
-    <col min="95" max="95" width="9.140625" style="1"/>
-    <col min="96" max="96" width="11.5703125" style="1" customWidth="1"/>
-    <col min="97" max="97" width="12.28515625" style="1" customWidth="1"/>
-    <col min="98" max="100" width="13.5703125" style="1" customWidth="1"/>
-    <col min="101" max="102" width="10.85546875" style="1" customWidth="1"/>
-    <col min="103" max="103" width="15.42578125" style="1" customWidth="1"/>
-    <col min="104" max="104" width="9.28515625" style="1"/>
-    <col min="105" max="105" width="17.7109375" style="1" customWidth="1"/>
-    <col min="106" max="106" width="17" style="1" customWidth="1"/>
-    <col min="107" max="107" width="17.7109375" style="1" customWidth="1"/>
-    <col min="108" max="108" width="12.28515625" style="1" customWidth="1"/>
-    <col min="109" max="109" width="17.7109375" style="1" customWidth="1"/>
-    <col min="110" max="110" width="11.7109375" style="1" customWidth="1"/>
+    <col min="63" max="63" width="22.7109375" style="1"/>
+    <col min="64" max="64" width="15.28515625" style="1" customWidth="1"/>
+    <col min="65" max="65" width="13" style="1" customWidth="1"/>
+    <col min="66" max="66" width="15.42578125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="22.7109375" style="1"/>
+    <col min="68" max="68" width="15.28515625" style="1" customWidth="1"/>
+    <col min="69" max="69" width="9.140625" style="1"/>
+    <col min="70" max="70" width="15.140625" style="1" customWidth="1"/>
+    <col min="71" max="71" width="20.140625" style="1" customWidth="1"/>
+    <col min="72" max="72" width="15.28515625" style="1" customWidth="1"/>
+    <col min="73" max="73" width="12.85546875" style="1" customWidth="1"/>
+    <col min="74" max="74" width="15.140625" style="1" customWidth="1"/>
+    <col min="75" max="75" width="20.140625" style="1" customWidth="1"/>
+    <col min="76" max="76" width="15.28515625" style="1" customWidth="1"/>
+    <col min="77" max="77" width="12.85546875" style="1" customWidth="1"/>
+    <col min="78" max="78" width="15.140625" style="1" customWidth="1"/>
+    <col min="79" max="79" width="20.140625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="15.28515625" style="1" customWidth="1"/>
+    <col min="81" max="81" width="12.85546875" style="1" customWidth="1"/>
+    <col min="82" max="82" width="9.140625" style="1"/>
+    <col min="83" max="83" width="11.42578125" style="1" customWidth="1"/>
+    <col min="84" max="84" width="15.28515625" style="1" customWidth="1"/>
+    <col min="85" max="86" width="9.140625" style="1"/>
+    <col min="87" max="87" width="11.42578125" style="1" customWidth="1"/>
+    <col min="88" max="88" width="15.28515625" style="1" customWidth="1"/>
+    <col min="89" max="91" width="9.140625" style="1"/>
+    <col min="92" max="92" width="15.28515625" style="1" customWidth="1"/>
+    <col min="93" max="95" width="9.140625" style="1"/>
+    <col min="96" max="96" width="15.28515625" style="1" customWidth="1"/>
+    <col min="97" max="99" width="9.140625" style="1"/>
+    <col min="100" max="100" width="15.28515625" style="1" customWidth="1"/>
+    <col min="101" max="101" width="9.140625" style="1"/>
+    <col min="102" max="102" width="11.5703125" style="1" customWidth="1"/>
+    <col min="103" max="103" width="12.28515625" style="1" customWidth="1"/>
+    <col min="104" max="106" width="13.5703125" style="1" customWidth="1"/>
+    <col min="107" max="108" width="10.85546875" style="1" customWidth="1"/>
+    <col min="109" max="109" width="15.42578125" style="1" customWidth="1"/>
+    <col min="110" max="110" width="9.28515625" style="1"/>
     <col min="111" max="111" width="17.7109375" style="1" customWidth="1"/>
-    <col min="112" max="112" width="16" style="1" customWidth="1"/>
+    <col min="112" max="112" width="17" style="1" customWidth="1"/>
     <col min="113" max="113" width="17.7109375" style="1" customWidth="1"/>
-    <col min="114" max="114" width="9.140625" style="1"/>
+    <col min="114" max="114" width="12.28515625" style="1" customWidth="1"/>
     <col min="115" max="115" width="17.7109375" style="1" customWidth="1"/>
-    <col min="116" max="116" width="12" customWidth="1"/>
+    <col min="116" max="116" width="11.7109375" style="1" customWidth="1"/>
     <col min="117" max="117" width="17.7109375" style="1" customWidth="1"/>
-    <col min="118" max="118" width="11.85546875" style="1" customWidth="1"/>
+    <col min="118" max="118" width="16" style="1" customWidth="1"/>
     <col min="119" max="119" width="17.7109375" style="1" customWidth="1"/>
-    <col min="120" max="120" width="11.85546875" style="1" customWidth="1"/>
+    <col min="120" max="120" width="9.140625" style="1"/>
     <col min="121" max="121" width="17.7109375" style="1" customWidth="1"/>
-    <col min="122" max="122" width="11.85546875" style="1" customWidth="1"/>
+    <col min="122" max="122" width="12" customWidth="1"/>
     <col min="123" max="123" width="17.7109375" style="1" customWidth="1"/>
     <col min="124" max="124" width="11.85546875" style="1" customWidth="1"/>
     <col min="125" max="125" width="17.7109375" style="1" customWidth="1"/>
     <col min="126" max="126" width="11.85546875" style="1" customWidth="1"/>
     <col min="127" max="127" width="17.7109375" style="1" customWidth="1"/>
-    <col min="128" max="128" width="14.85546875" style="1" customWidth="1"/>
+    <col min="128" max="128" width="11.85546875" style="1" customWidth="1"/>
     <col min="129" max="129" width="17.7109375" style="1" customWidth="1"/>
-    <col min="130" max="130" width="12.28515625" style="1" customWidth="1"/>
+    <col min="130" max="130" width="11.85546875" style="1" customWidth="1"/>
     <col min="131" max="131" width="17.7109375" style="1" customWidth="1"/>
-    <col min="132" max="132" width="9.140625" style="1"/>
+    <col min="132" max="132" width="11.85546875" style="1" customWidth="1"/>
     <col min="133" max="133" width="17.7109375" style="1" customWidth="1"/>
-    <col min="134" max="134" width="9.140625" style="1"/>
+    <col min="134" max="134" width="14.85546875" style="1" customWidth="1"/>
     <col min="135" max="135" width="17.7109375" style="1" customWidth="1"/>
-    <col min="136" max="136" width="18.42578125" style="1" customWidth="1"/>
+    <col min="136" max="136" width="12.28515625" style="1" customWidth="1"/>
     <col min="137" max="137" width="17.7109375" style="1" customWidth="1"/>
-    <col min="138" max="138" width="10.140625" style="1" customWidth="1"/>
+    <col min="138" max="138" width="9.140625" style="1"/>
     <col min="139" max="139" width="17.7109375" style="1" customWidth="1"/>
-    <col min="140" max="1127" width="9.28515625" style="1"/>
+    <col min="140" max="140" width="9.140625" style="1"/>
+    <col min="141" max="141" width="17.7109375" style="1" customWidth="1"/>
+    <col min="142" max="142" width="18.42578125" style="1" customWidth="1"/>
+    <col min="143" max="143" width="17.7109375" style="1" customWidth="1"/>
+    <col min="144" max="144" width="10.140625" style="1" customWidth="1"/>
+    <col min="145" max="145" width="17.7109375" style="1" customWidth="1"/>
+    <col min="146" max="1133" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:139" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:145" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:139" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:145" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -2304,98 +2316,98 @@
       <c r="AD2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AE2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AM2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="21" t="s">
+      <c r="AN2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AI2" s="51" t="s">
+      <c r="AO2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AJ2" s="51" t="s">
+      <c r="AP2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AK2" s="21" t="s">
+      <c r="AQ2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AL2" s="51" t="s">
+      <c r="AR2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AM2" s="12" t="s">
+      <c r="AS2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AN2" s="12" t="s">
+      <c r="AT2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AO2" s="12" t="s">
+      <c r="AU2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AV2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AQ2" s="12" t="s">
+      <c r="AW2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AR2" s="12" t="s">
+      <c r="AX2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AS2" s="20" t="s">
+      <c r="AY2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AT2" s="20" t="s">
+      <c r="AZ2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AU2" s="51" t="s">
+      <c r="BA2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AV2" s="21" t="s">
+      <c r="BB2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AW2" s="51" t="s">
+      <c r="BC2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AX2" s="51" t="s">
+      <c r="BD2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AY2" s="21" t="s">
+      <c r="BE2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AZ2" s="51" t="s">
+      <c r="BF2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="BA2" s="22" t="s">
+      <c r="BG2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="BB2" s="22" t="s">
+      <c r="BH2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="BC2" s="23" t="s">
+      <c r="BI2" s="23" t="s">
         <v>41</v>
-      </c>
-      <c r="BD2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="BE2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="BF2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="BG2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="BH2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="19" t="s">
-        <v>1</v>
       </c>
       <c r="BJ2" s="48" t="s">
         <v>1</v>
@@ -2403,119 +2415,119 @@
       <c r="BK2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BL2" s="19" t="s">
+      <c r="BL2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BM2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BN2" s="48" t="s">
+      <c r="BN2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BO2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BP2" s="19" t="s">
+      <c r="BP2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BQ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BR2" s="48" t="s">
+      <c r="BR2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BS2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BT2" s="19" t="s">
+      <c r="BT2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BU2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BV2" s="48" t="s">
+      <c r="BV2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="BW2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BX2" s="19" t="s">
+      <c r="BX2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BY2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BZ2" s="48" t="s">
+      <c r="BZ2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="CA2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CB2" s="19" t="s">
+      <c r="CB2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CC2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CD2" s="48" t="s">
+      <c r="CD2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="CE2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CF2" s="19" t="s">
+      <c r="CF2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CG2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CH2" s="48" t="s">
+      <c r="CH2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="CI2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CJ2" s="19" t="s">
+      <c r="CJ2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CK2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CL2" s="48" t="s">
+      <c r="CL2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="CM2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CN2" s="19" t="s">
+      <c r="CN2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CO2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CP2" s="48" t="s">
+      <c r="CP2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="CQ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CR2" s="19" t="s">
-        <v>120</v>
+      <c r="CR2" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="CS2" s="19" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="CT2" s="19" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="CU2" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="CV2" s="19" t="s">
-        <v>120</v>
+        <v>1</v>
+      </c>
+      <c r="CV2" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="CW2" s="19" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="CX2" s="19" t="s">
         <v>120</v>
@@ -2523,23 +2535,23 @@
       <c r="CY2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="CZ2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="DA2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="DB2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="DC2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="DD2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="DE2" s="29" t="s">
-        <v>65</v>
+      <c r="CZ2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="DA2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="DB2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="DC2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="DD2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="DE2" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="DF2" s="29" t="s">
         <v>65</v>
@@ -2547,7 +2559,7 @@
       <c r="DG2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="DH2" s="28" t="s">
+      <c r="DH2" s="29" t="s">
         <v>65</v>
       </c>
       <c r="DI2" s="29" t="s">
@@ -2565,7 +2577,7 @@
       <c r="DM2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="DN2" s="29" t="s">
+      <c r="DN2" s="28" t="s">
         <v>65</v>
       </c>
       <c r="DO2" s="29" t="s">
@@ -2595,7 +2607,7 @@
       <c r="DW2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="DX2" s="30" t="s">
+      <c r="DX2" s="29" t="s">
         <v>65</v>
       </c>
       <c r="DY2" s="29" t="s">
@@ -2613,7 +2625,7 @@
       <c r="EC2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="ED2" s="29" t="s">
+      <c r="ED2" s="30" t="s">
         <v>65</v>
       </c>
       <c r="EE2" s="29" t="s">
@@ -2631,8 +2643,26 @@
       <c r="EI2" s="29" t="s">
         <v>65</v>
       </c>
+      <c r="EJ2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EK2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EL2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EM2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EN2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EO2" s="29" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="3" spans="1:139" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:145" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>68</v>
       </c>
@@ -2721,335 +2751,353 @@
       <c r="AD3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="AE3" s="49" t="s">
+      <c r="AE3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK3" s="49" t="s">
         <v>204</v>
       </c>
-      <c r="AF3" s="49" t="s">
+      <c r="AL3" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="AG3" s="54" t="s">
+      <c r="AM3" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="AH3" s="13" t="s">
+      <c r="AN3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AI3" s="52" t="s">
+      <c r="AO3" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="AJ3" s="52" t="s">
+      <c r="AP3" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="AK3" s="13" t="s">
+      <c r="AQ3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="AL3" s="52" t="s">
+      <c r="AR3" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="AM3" s="11" t="s">
+      <c r="AS3" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="AN3" s="11" t="s">
+      <c r="AT3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AO3" s="11" t="s">
+      <c r="AU3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AP3" s="10" t="s">
+      <c r="AV3" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="AQ3" s="10" t="s">
+      <c r="AW3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="AR3" s="37" t="s">
+      <c r="AX3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="AS3" s="49" t="s">
+      <c r="AY3" s="49" t="s">
         <v>204</v>
       </c>
-      <c r="AT3" s="49" t="s">
+      <c r="AZ3" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="AU3" s="54" t="s">
+      <c r="BA3" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="AV3" s="13" t="s">
+      <c r="BB3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AW3" s="52" t="s">
+      <c r="BC3" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="AX3" s="52" t="s">
+      <c r="BD3" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="AY3" s="13" t="s">
+      <c r="BE3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="AZ3" s="52" t="s">
+      <c r="BF3" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="BA3" s="24" t="s">
+      <c r="BG3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BB3" s="25" t="s">
+      <c r="BH3" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="BC3" s="24" t="s">
+      <c r="BI3" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="BD3" s="27" t="s">
+      <c r="BJ3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BE3" s="27" t="s">
+      <c r="BK3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BF3" s="27" t="s">
+      <c r="BL3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BG3" s="27" t="s">
+      <c r="BM3" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="BH3" s="27" t="s">
+      <c r="BN3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BI3" s="27" t="s">
+      <c r="BO3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BJ3" s="27" t="s">
+      <c r="BP3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BK3" s="27" t="s">
+      <c r="BQ3" s="27" t="s">
         <v>295</v>
       </c>
-      <c r="BL3" s="27" t="s">
+      <c r="BR3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BM3" s="27" t="s">
+      <c r="BS3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BN3" s="27" t="s">
+      <c r="BT3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BO3" s="27" t="s">
+      <c r="BU3" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="BP3" s="27" t="s">
+      <c r="BV3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BQ3" s="27" t="s">
+      <c r="BW3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BR3" s="27" t="s">
+      <c r="BX3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BS3" s="27" t="s">
+      <c r="BY3" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="BT3" s="27" t="s">
+      <c r="BZ3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BU3" s="27" t="s">
+      <c r="CA3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BV3" s="27" t="s">
+      <c r="CB3" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="BW3" s="27" t="s">
+      <c r="CC3" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="BX3" s="27" t="s">
+      <c r="CD3" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="BY3" s="27" t="s">
+      <c r="CE3" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="BZ3" s="27" t="s">
+      <c r="CF3" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="CA3" s="27" t="s">
+      <c r="CG3" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="CB3" s="27" t="s">
+      <c r="CH3" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="CC3" s="27" t="s">
+      <c r="CI3" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="CD3" s="27" t="s">
+      <c r="CJ3" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="CE3" s="27" t="s">
+      <c r="CK3" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="CF3" s="27" t="s">
+      <c r="CL3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="CG3" s="27" t="s">
+      <c r="CM3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="CH3" s="27" t="s">
+      <c r="CN3" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="CI3" s="27" t="s">
+      <c r="CO3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="CJ3" s="27" t="s">
+      <c r="CP3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="CK3" s="27" t="s">
+      <c r="CQ3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="CL3" s="27" t="s">
+      <c r="CR3" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="CM3" s="27" t="s">
+      <c r="CS3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="CN3" s="27" t="s">
+      <c r="CT3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="CO3" s="27" t="s">
+      <c r="CU3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="CP3" s="27" t="s">
+      <c r="CV3" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="CQ3" s="27" t="s">
+      <c r="CW3" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="CR3" s="27" t="s">
+      <c r="CX3" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="CS3" s="27" t="s">
+      <c r="CY3" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="CT3" s="27" t="s">
+      <c r="CZ3" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="CU3" s="27" t="s">
+      <c r="DA3" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="CV3" s="27" t="s">
+      <c r="DB3" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="CW3" s="27" t="s">
+      <c r="DC3" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="CX3" s="27" t="s">
+      <c r="DD3" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="CY3" s="27" t="s">
+      <c r="DE3" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="CZ3" s="26" t="s">
+      <c r="DF3" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="DA3" s="59" t="s">
+      <c r="DG3" s="59" t="s">
         <v>246</v>
       </c>
-      <c r="DB3" s="26" t="s">
+      <c r="DH3" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="DC3" s="59" t="s">
+      <c r="DI3" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="DD3" s="26" t="s">
+      <c r="DJ3" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="DE3" s="59" t="s">
+      <c r="DK3" s="59" t="s">
         <v>242</v>
       </c>
-      <c r="DF3" s="26" t="s">
+      <c r="DL3" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="DG3" s="59" t="s">
+      <c r="DM3" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="DH3" s="26" t="s">
+      <c r="DN3" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="DI3" s="59" t="s">
+      <c r="DO3" s="59" t="s">
         <v>238</v>
       </c>
-      <c r="DJ3" s="26" t="s">
+      <c r="DP3" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="DK3" s="59" t="s">
+      <c r="DQ3" s="59" t="s">
         <v>236</v>
       </c>
-      <c r="DL3" s="26" t="s">
+      <c r="DR3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="DM3" s="59" t="s">
+      <c r="DS3" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="DN3" s="26" t="s">
+      <c r="DT3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DO3" s="59" t="s">
+      <c r="DU3" s="59" t="s">
         <v>232</v>
       </c>
-      <c r="DP3" s="26" t="s">
+      <c r="DV3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="DQ3" s="59" t="s">
+      <c r="DW3" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="DR3" s="26" t="s">
+      <c r="DX3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DS3" s="59" t="s">
+      <c r="DY3" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="DT3" s="26" t="s">
+      <c r="DZ3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="DU3" s="59" t="s">
+      <c r="EA3" s="59" t="s">
         <v>226</v>
       </c>
-      <c r="DV3" s="26" t="s">
+      <c r="EB3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="DW3" s="59" t="s">
+      <c r="EC3" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="DX3" s="26" t="s">
+      <c r="ED3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="DY3" s="59" t="s">
+      <c r="EE3" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="DZ3" s="26" t="s">
+      <c r="EF3" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="EA3" s="59" t="s">
+      <c r="EG3" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="EB3" s="26" t="s">
+      <c r="EH3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="EC3" s="59" t="s">
+      <c r="EI3" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="ED3" s="26" t="s">
+      <c r="EJ3" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="EE3" s="59" t="s">
+      <c r="EK3" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="EF3" s="26" t="s">
+      <c r="EL3" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="EG3" s="59" t="s">
+      <c r="EM3" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="EH3" s="26" t="s">
+      <c r="EN3" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="EI3" s="59" t="s">
+      <c r="EO3" s="59" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:139" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:145" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
@@ -3141,334 +3189,352 @@
         <v>37</v>
       </c>
       <c r="AE4" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="AF4" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="AG4" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="AH4" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="AI4" s="38" t="s">
+        <v>365</v>
+      </c>
+      <c r="AJ4" s="41" t="s">
+        <v>367</v>
+      </c>
+      <c r="AK4" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="AF4" s="38" t="s">
+      <c r="AL4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AG4" s="40" t="s">
+      <c r="AM4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AH4" s="38" t="s">
+      <c r="AN4" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AI4" s="40" t="s">
+      <c r="AO4" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AJ4" s="40" t="s">
+      <c r="AP4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="AK4" s="38" t="s">
+      <c r="AQ4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="AL4" s="40" t="s">
+      <c r="AR4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="AM4" s="38" t="s">
+      <c r="AS4" s="38" t="s">
         <v>358</v>
       </c>
-      <c r="AN4" s="38" t="s">
+      <c r="AT4" s="38" t="s">
         <v>359</v>
       </c>
-      <c r="AO4" s="38" t="s">
+      <c r="AU4" s="38" t="s">
         <v>361</v>
       </c>
-      <c r="AP4" s="38" t="s">
+      <c r="AV4" s="38" t="s">
         <v>363</v>
       </c>
-      <c r="AQ4" s="38" t="s">
+      <c r="AW4" s="38" t="s">
         <v>365</v>
       </c>
-      <c r="AR4" s="61" t="s">
+      <c r="AX4" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="AS4" s="38" t="s">
+      <c r="AY4" s="38" t="s">
         <v>369</v>
       </c>
-      <c r="AT4" s="38" t="s">
+      <c r="AZ4" s="38" t="s">
         <v>371</v>
       </c>
-      <c r="AU4" s="40" t="s">
+      <c r="BA4" s="40" t="s">
         <v>373</v>
       </c>
-      <c r="AV4" s="38" t="s">
+      <c r="BB4" s="38" t="s">
         <v>376</v>
       </c>
-      <c r="AW4" s="40" t="s">
+      <c r="BC4" s="40" t="s">
         <v>377</v>
       </c>
-      <c r="AX4" s="40" t="s">
+      <c r="BD4" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="AY4" s="38" t="s">
+      <c r="BE4" s="38" t="s">
         <v>381</v>
       </c>
-      <c r="AZ4" s="40" t="s">
+      <c r="BF4" s="40" t="s">
         <v>383</v>
       </c>
-      <c r="BA4" s="38" t="s">
+      <c r="BG4" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="BB4" s="38" t="s">
+      <c r="BH4" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="BC4" s="38" t="s">
+      <c r="BI4" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="BD4" s="38" t="s">
+      <c r="BJ4" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="BE4" s="38" t="s">
+      <c r="BK4" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="BF4" s="38" t="s">
+      <c r="BL4" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="BG4" s="38" t="s">
+      <c r="BM4" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="BH4" s="38" t="s">
+      <c r="BN4" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="BI4" s="38" t="s">
+      <c r="BO4" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="BJ4" s="38" t="s">
+      <c r="BP4" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="BK4" s="38" t="s">
+      <c r="BQ4" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="BL4" s="38" t="s">
+      <c r="BR4" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="BM4" s="38" t="s">
+      <c r="BS4" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="BN4" s="38" t="s">
+      <c r="BT4" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="BO4" s="38" t="s">
+      <c r="BU4" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="BP4" s="38" t="s">
+      <c r="BV4" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="BQ4" s="38" t="s">
+      <c r="BW4" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="BR4" s="38" t="s">
+      <c r="BX4" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="BS4" s="38" t="s">
+      <c r="BY4" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="BT4" s="38" t="s">
+      <c r="BZ4" s="38" t="s">
         <v>328</v>
       </c>
-      <c r="BU4" s="38" t="s">
+      <c r="CA4" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="BV4" s="38" t="s">
+      <c r="CB4" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="BW4" s="38" t="s">
+      <c r="CC4" s="38" t="s">
         <v>334</v>
       </c>
-      <c r="BX4" s="38" t="s">
+      <c r="CD4" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="BY4" s="38" t="s">
+      <c r="CE4" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="BZ4" s="38" t="s">
+      <c r="CF4" s="38" t="s">
         <v>287</v>
       </c>
-      <c r="CA4" s="38" t="s">
+      <c r="CG4" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="CB4" s="38" t="s">
+      <c r="CH4" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="CC4" s="38" t="s">
+      <c r="CI4" s="38" t="s">
         <v>303</v>
       </c>
-      <c r="CD4" s="38" t="s">
+      <c r="CJ4" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="CE4" s="38" t="s">
+      <c r="CK4" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="CF4" s="38" t="s">
+      <c r="CL4" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="CG4" s="38" t="s">
+      <c r="CM4" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="CH4" s="38" t="s">
+      <c r="CN4" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="CI4" s="38" t="s">
+      <c r="CO4" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="CJ4" s="38" t="s">
+      <c r="CP4" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="CK4" s="38" t="s">
+      <c r="CQ4" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="CL4" s="38" t="s">
+      <c r="CR4" s="38" t="s">
         <v>292</v>
       </c>
-      <c r="CM4" s="38" t="s">
+      <c r="CS4" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="CN4" s="38" t="s">
+      <c r="CT4" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="CO4" s="38" t="s">
+      <c r="CU4" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="CP4" s="38" t="s">
+      <c r="CV4" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="CQ4" s="38" t="s">
+      <c r="CW4" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="CR4" s="38" t="s">
+      <c r="CX4" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="CS4" s="38" t="s">
+      <c r="CY4" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="CT4" s="38" t="s">
+      <c r="CZ4" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="CU4" s="38" t="s">
+      <c r="DA4" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="CV4" s="38" t="s">
+      <c r="DB4" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="CW4" s="38" t="s">
+      <c r="DC4" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="CX4" s="38" t="s">
+      <c r="DD4" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="CY4" s="38" t="s">
+      <c r="DE4" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="CZ4" s="38" t="s">
+      <c r="DF4" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="DA4" s="38" t="s">
+      <c r="DG4" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="DB4" s="38" t="s">
+      <c r="DH4" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="DC4" s="38" t="s">
+      <c r="DI4" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="DD4" s="41" t="s">
+      <c r="DJ4" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="DE4" s="38" t="s">
+      <c r="DK4" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="DF4" s="38" t="s">
+      <c r="DL4" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="DG4" s="38" t="s">
+      <c r="DM4" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="DH4" s="38" t="s">
+      <c r="DN4" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="DI4" s="38" t="s">
+      <c r="DO4" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="DJ4" s="41" t="s">
+      <c r="DP4" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="DK4" s="38" t="s">
+      <c r="DQ4" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="DL4" s="41" t="s">
+      <c r="DR4" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="DM4" s="38" t="s">
+      <c r="DS4" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="DN4" s="41" t="s">
+      <c r="DT4" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="DO4" s="38" t="s">
+      <c r="DU4" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="DP4" s="41" t="s">
+      <c r="DV4" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="DQ4" s="38" t="s">
+      <c r="DW4" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="DR4" s="38" t="s">
+      <c r="DX4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="DS4" s="38" t="s">
+      <c r="DY4" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="DT4" s="38" t="s">
+      <c r="DZ4" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="DU4" s="38" t="s">
+      <c r="EA4" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="DV4" s="38" t="s">
+      <c r="EB4" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="DW4" s="38" t="s">
+      <c r="EC4" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="DX4" s="41" t="s">
+      <c r="ED4" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="DY4" s="38" t="s">
+      <c r="EE4" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="DZ4" s="38" t="s">
+      <c r="EF4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="EA4" s="38" t="s">
+      <c r="EG4" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="EB4" s="41" t="s">
+      <c r="EH4" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="EC4" s="38" t="s">
+      <c r="EI4" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="ED4" s="38" t="s">
+      <c r="EJ4" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="EE4" s="38" t="s">
+      <c r="EK4" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="EF4" s="41" t="s">
+      <c r="EL4" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="EG4" s="41" t="s">
+      <c r="EM4" s="41" t="s">
         <v>264</v>
       </c>
-      <c r="EH4" s="41" t="s">
+      <c r="EN4" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="EI4" s="38" t="s">
+      <c r="EO4" s="38" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:139" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:145" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>67</v>
       </c>
@@ -3560,335 +3626,353 @@
         <v>4</v>
       </c>
       <c r="AE5" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="AG5" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="AK5" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AL5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG5" s="53" t="s">
+      <c r="AM5" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI5" s="53" t="s">
+      <c r="AO5" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="AJ5" s="53" t="s">
+      <c r="AP5" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="53" t="s">
+      <c r="AR5" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AS5" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="AN5" s="6" t="s">
+      <c r="AT5" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="AO5" s="6" t="s">
+      <c r="AU5" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AV5" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="AW5" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="AX5" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="AS5" s="4" t="s">
+      <c r="AY5" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="AT5" s="4" t="s">
+      <c r="AZ5" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="AU5" s="53" t="s">
+      <c r="BA5" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="AV5" s="4" t="s">
+      <c r="BB5" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="AW5" s="53" t="s">
+      <c r="BC5" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="AX5" s="53" t="s">
+      <c r="BD5" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="AY5" s="4" t="s">
+      <c r="BE5" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="AZ5" s="53" t="s">
+      <c r="BF5" s="53" t="s">
         <v>384</v>
       </c>
-      <c r="BA5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="BB5" s="4" t="s">
+      <c r="BH5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="BC5" s="4" t="s">
+      <c r="BI5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="BD5" s="4" t="s">
+      <c r="BJ5" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="BE5" s="4" t="s">
+      <c r="BK5" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="BF5" s="4" t="s">
+      <c r="BL5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="BG5" s="4" t="s">
+      <c r="BM5" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="BH5" s="4" t="s">
+      <c r="BN5" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="BI5" s="4" t="s">
+      <c r="BO5" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="BJ5" s="4" t="s">
+      <c r="BP5" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="BK5" s="4" t="s">
+      <c r="BQ5" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="BL5" s="4" t="s">
+      <c r="BR5" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="BM5" s="4" t="s">
+      <c r="BS5" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="BN5" s="4" t="s">
+      <c r="BT5" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="BO5" s="4" t="s">
+      <c r="BU5" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="BP5" s="4" t="s">
+      <c r="BV5" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="BQ5" s="4" t="s">
+      <c r="BW5" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="BR5" s="4" t="s">
+      <c r="BX5" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="BS5" s="4" t="s">
+      <c r="BY5" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="BT5" s="4" t="s">
+      <c r="BZ5" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="BU5" s="4" t="s">
+      <c r="CA5" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="BV5" s="4" t="s">
+      <c r="CB5" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="BW5" s="4" t="s">
+      <c r="CC5" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="BX5" s="4" t="s">
+      <c r="CD5" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="BY5" s="4" t="s">
+      <c r="CE5" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="BZ5" s="4" t="s">
+      <c r="CF5" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="CA5" s="4" t="s">
+      <c r="CG5" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="CB5" s="4" t="s">
+      <c r="CH5" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="CC5" s="4" t="s">
+      <c r="CI5" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="CD5" s="4" t="s">
+      <c r="CJ5" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="CE5" s="4" t="s">
+      <c r="CK5" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="CF5" s="4" t="s">
+      <c r="CL5" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="CG5" s="4" t="s">
+      <c r="CM5" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="CH5" s="4" t="s">
+      <c r="CN5" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="CI5" s="4" t="s">
+      <c r="CO5" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="CJ5" s="4" t="s">
+      <c r="CP5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="CK5" s="4" t="s">
+      <c r="CQ5" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="CL5" s="4" t="s">
+      <c r="CR5" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="CM5" s="4" t="s">
+      <c r="CS5" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="CN5" s="4" t="s">
+      <c r="CT5" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="CO5" s="4" t="s">
+      <c r="CU5" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="CP5" s="4" t="s">
+      <c r="CV5" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="CQ5" s="4" t="s">
+      <c r="CW5" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="CR5" s="4" t="s">
+      <c r="CX5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="CS5" s="4" t="s">
+      <c r="CY5" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="CT5" s="4" t="s">
+      <c r="CZ5" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="CU5" s="4" t="s">
+      <c r="DA5" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="CV5" s="4" t="s">
+      <c r="DB5" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="CW5" s="4" t="s">
+      <c r="DC5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="CX5" s="4" t="s">
+      <c r="DD5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="CY5" s="4" t="s">
+      <c r="DE5" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="CZ5" s="4" t="s">
+      <c r="DF5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="DA5" s="4" t="s">
+      <c r="DG5" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="DB5" s="4" t="s">
+      <c r="DH5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="DC5" s="4" t="s">
+      <c r="DI5" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="DD5" s="7" t="s">
+      <c r="DJ5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="DE5" s="4" t="s">
+      <c r="DK5" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="DF5" s="4" t="s">
+      <c r="DL5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="DG5" s="4" t="s">
+      <c r="DM5" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="DH5" s="4" t="s">
+      <c r="DN5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="DI5" s="4" t="s">
+      <c r="DO5" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="DJ5" s="7" t="s">
+      <c r="DP5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="DK5" s="4" t="s">
+      <c r="DQ5" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="DL5" s="7" t="s">
+      <c r="DR5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="DM5" s="4" t="s">
+      <c r="DS5" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="DN5" s="7" t="s">
+      <c r="DT5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="DO5" s="4" t="s">
+      <c r="DU5" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="DP5" s="7" t="s">
+      <c r="DV5" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="DQ5" s="4" t="s">
+      <c r="DW5" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="DR5" s="4" t="s">
+      <c r="DX5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="DS5" s="4" t="s">
+      <c r="DY5" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="DT5" s="4" t="s">
+      <c r="DZ5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="DU5" s="4" t="s">
+      <c r="EA5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="DV5" s="4" t="s">
+      <c r="EB5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="DW5" s="4" t="s">
+      <c r="EC5" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="DX5" s="14" t="s">
+      <c r="ED5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="DY5" s="4" t="s">
+      <c r="EE5" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="DZ5" s="4" t="s">
+      <c r="EF5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="EA5" s="4" t="s">
+      <c r="EG5" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="EB5" s="7" t="s">
+      <c r="EH5" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="EC5" s="4" t="s">
+      <c r="EI5" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="ED5" s="4" t="s">
+      <c r="EJ5" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="EE5" s="4" t="s">
+      <c r="EK5" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="EF5" s="7" t="s">
+      <c r="EL5" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="EG5" s="4" t="s">
+      <c r="EM5" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="EH5" s="7" t="s">
+      <c r="EN5" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="EI5" s="4" t="s">
+      <c r="EO5" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:139" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:145" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:145" x14ac:dyDescent="0.25">
       <c r="G7" s="32"/>
     </row>
   </sheetData>
@@ -3906,7 +3990,7 @@
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 EG6:EG1048576 EE6:EE1048576 EI6:EI1048576 EC6:EC1048576 EA6:EA1048576 DY6:DY1048576 DW6:DW1048576 DU6:DU1048576 DS6:DS1048576 DQ6:DQ1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 DI6:DI1048576 DG6:DG1048576 DE6:DE1048576 DC6:DC1048576 DA6:DA1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 EM6:EM1048576 EK6:EK1048576 EO6:EO1048576 EI6:EI1048576 EG6:EG1048576 EE6:EE1048576 EC6:EC1048576 EA6:EA1048576 DY6:DY1048576 DW6:DW1048576 DU6:DU1048576 DS6:DS1048576 DQ6:DQ1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 DI6:DI1048576 DG6:DG1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3919,7 +4003,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>BF6:BF1048576 BJ6:BJ1048576 BZ6:BZ1048576 BN6:BN1048576 CL6:CL1048576 CD6:CD1048576 CH6:CH1048576 CP6:CP1048576 BR6:BR1048576 BV6:BV1048576</xm:sqref>
+          <xm:sqref>BL6:BL1048576 BP6:BP1048576 CF6:CF1048576 BT6:BT1048576 CR6:CR1048576 CJ6:CJ1048576 CN6:CN1048576 CV6:CV1048576 BX6:BX1048576 CB6:CB1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
rearrange extension and container columns
</commit_message>
<xml_diff>
--- a/templates/extended_aspace_import_excel_template.xlsx
+++ b/templates/extended_aspace_import_excel_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbi\Documents\aspace\archivesspace_2_5_1\plugins\aspace-import-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2546B4AF-2B90-4DC7-A327-55A0C433BFD9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CEDA04-BFD6-4AD9-9FBC-FF14CEAF88A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1200" windowWidth="20085" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="615" windowWidth="20910" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2083,9 +2083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AE1:AJ1048576"/>
+      <selection pane="bottomLeft" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,15 +2113,15 @@
     <col min="21" max="21" width="10.5703125" style="50" customWidth="1"/>
     <col min="22" max="22" width="23.85546875" style="1" customWidth="1"/>
     <col min="23" max="23" width="15.140625" style="50" customWidth="1"/>
-    <col min="24" max="31" width="26.85546875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="23" style="1"/>
-    <col min="33" max="33" width="23" style="50"/>
-    <col min="34" max="34" width="10.42578125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="19" style="50" customWidth="1"/>
-    <col min="36" max="36" width="19.140625" style="50" customWidth="1"/>
-    <col min="37" max="37" width="10.42578125" style="1" customWidth="1"/>
-    <col min="38" max="38" width="11.42578125" style="50" customWidth="1"/>
-    <col min="39" max="45" width="26.85546875" style="1" customWidth="1"/>
+    <col min="24" max="37" width="26.85546875" style="1" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" style="1"/>
+    <col min="39" max="39" width="9.140625" style="50"/>
+    <col min="40" max="40" width="10.42578125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="19" style="50" customWidth="1"/>
+    <col min="42" max="42" width="19.140625" style="50" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="11.42578125" style="50" customWidth="1"/>
+    <col min="45" max="45" width="26.85546875" style="1" customWidth="1"/>
     <col min="46" max="46" width="9.140625" style="1"/>
     <col min="47" max="47" width="9.140625" style="50"/>
     <col min="48" max="48" width="10.42578125" style="1" customWidth="1"/>
@@ -2304,47 +2304,47 @@
       <c r="AD2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AE2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AM2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="21" t="s">
+      <c r="AN2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AI2" s="51" t="s">
+      <c r="AO2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AJ2" s="51" t="s">
+      <c r="AP2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AK2" s="21" t="s">
+      <c r="AQ2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AL2" s="51" t="s">
+      <c r="AR2" s="51" t="s">
         <v>30</v>
-      </c>
-      <c r="AM2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AR2" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="AS2" s="20" t="s">
         <v>30</v>
@@ -2721,47 +2721,47 @@
       <c r="AD3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="AE3" s="49" t="s">
+      <c r="AE3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK3" s="49" t="s">
         <v>204</v>
       </c>
-      <c r="AF3" s="49" t="s">
+      <c r="AL3" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="AG3" s="54" t="s">
+      <c r="AM3" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="AH3" s="13" t="s">
+      <c r="AN3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AI3" s="52" t="s">
+      <c r="AO3" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="AJ3" s="52" t="s">
+      <c r="AP3" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="AK3" s="13" t="s">
+      <c r="AQ3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="AL3" s="52" t="s">
+      <c r="AR3" s="52" t="s">
         <v>93</v>
-      </c>
-      <c r="AM3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AP3" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="AQ3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="AR3" s="37" t="s">
-        <v>36</v>
       </c>
       <c r="AS3" s="49" t="s">
         <v>204</v>
@@ -3141,46 +3141,46 @@
         <v>37</v>
       </c>
       <c r="AE4" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="AF4" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="AG4" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="AH4" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="AI4" s="38" t="s">
+        <v>365</v>
+      </c>
+      <c r="AJ4" s="61" t="s">
+        <v>367</v>
+      </c>
+      <c r="AK4" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="AF4" s="38" t="s">
+      <c r="AL4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AG4" s="40" t="s">
+      <c r="AM4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AH4" s="38" t="s">
+      <c r="AN4" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AI4" s="40" t="s">
+      <c r="AO4" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AJ4" s="40" t="s">
+      <c r="AP4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="AK4" s="38" t="s">
+      <c r="AQ4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="AL4" s="40" t="s">
+      <c r="AR4" s="40" t="s">
         <v>34</v>
-      </c>
-      <c r="AM4" s="38" t="s">
-        <v>358</v>
-      </c>
-      <c r="AN4" s="38" t="s">
-        <v>359</v>
-      </c>
-      <c r="AO4" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="AP4" s="38" t="s">
-        <v>363</v>
-      </c>
-      <c r="AQ4" s="38" t="s">
-        <v>365</v>
-      </c>
-      <c r="AR4" s="61" t="s">
-        <v>367</v>
       </c>
       <c r="AS4" s="38" t="s">
         <v>369</v>
@@ -3560,46 +3560,46 @@
         <v>4</v>
       </c>
       <c r="AE5" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="AG5" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="AK5" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AL5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG5" s="53" t="s">
+      <c r="AM5" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI5" s="53" t="s">
+      <c r="AO5" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="AJ5" s="53" t="s">
+      <c r="AP5" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="53" t="s">
+      <c r="AR5" s="53" t="s">
         <v>91</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="AN5" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="AO5" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="AP5" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>368</v>
       </c>
       <c r="AS5" s="4" t="s">
         <v>370</v>

</xml_diff>

<commit_message>
get rid of old lang materials column
</commit_message>
<xml_diff>
--- a/templates/extended_aspace_import_excel_template.xlsx
+++ b/templates/extended_aspace_import_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlynn\Aspace\Compiled\archivesspace\plugins\aspace-import-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FF484F2-498F-4241-8184-9CAE305562E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8AB0CC-1A93-467F-B5AA-B3048FA8178F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="398">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -463,12 +463,6 @@
   </si>
   <si>
     <t>Note with Type=General</t>
-  </si>
-  <si>
-    <t>Language of Materials</t>
-  </si>
-  <si>
-    <t>Note with Type=Language of Materials</t>
   </si>
   <si>
     <t>Note with Type=Physical Description</t>
@@ -719,12 +713,6 @@
   </si>
   <si>
     <t>Publish Physical Description?</t>
-  </si>
-  <si>
-    <t>Publish Language of Materials?</t>
-  </si>
-  <si>
-    <t>Publish (true/false) Language of Materials</t>
   </si>
   <si>
     <t>Publish (true/false) General</t>
@@ -2160,11 +2148,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQQ7"/>
+  <dimension ref="A1:AQO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomLeft" activeCell="DY1" sqref="DX1:DY1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2273,29 +2261,27 @@
     <col min="131" max="131" width="17.68359375" style="1" customWidth="1"/>
     <col min="132" max="132" width="11.83984375" style="1" customWidth="1"/>
     <col min="133" max="133" width="17.68359375" style="1" customWidth="1"/>
-    <col min="134" max="134" width="11.83984375" style="1" customWidth="1"/>
+    <col min="134" max="134" width="14.83984375" style="1" customWidth="1"/>
     <col min="135" max="135" width="17.68359375" style="1" customWidth="1"/>
-    <col min="136" max="136" width="14.83984375" style="1" customWidth="1"/>
+    <col min="136" max="136" width="12.26171875" style="1" customWidth="1"/>
     <col min="137" max="137" width="17.68359375" style="1" customWidth="1"/>
-    <col min="138" max="138" width="12.26171875" style="1" customWidth="1"/>
+    <col min="138" max="138" width="9.15625" style="1"/>
     <col min="139" max="139" width="17.68359375" style="1" customWidth="1"/>
     <col min="140" max="140" width="9.15625" style="1"/>
     <col min="141" max="141" width="17.68359375" style="1" customWidth="1"/>
-    <col min="142" max="142" width="9.15625" style="1"/>
+    <col min="142" max="142" width="18.41796875" style="1" customWidth="1"/>
     <col min="143" max="143" width="17.68359375" style="1" customWidth="1"/>
-    <col min="144" max="144" width="18.41796875" style="1" customWidth="1"/>
+    <col min="144" max="144" width="10.15625" style="1" customWidth="1"/>
     <col min="145" max="145" width="17.68359375" style="1" customWidth="1"/>
-    <col min="146" max="146" width="10.15625" style="1" customWidth="1"/>
-    <col min="147" max="147" width="17.68359375" style="1" customWidth="1"/>
-    <col min="148" max="1135" width="9.26171875" style="1"/>
+    <col min="146" max="1133" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:147" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:145" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="31" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:147" s="1" customFormat="1" ht="51.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:145" s="1" customFormat="1" ht="51.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -2333,28 +2319,28 @@
         <v>99</v>
       </c>
       <c r="M2" s="63" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="N2" s="63" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="O2" s="63" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="P2" s="64" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="Q2" s="63" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="R2" s="63" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="S2" s="63" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="T2" s="64" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="U2" s="18" t="s">
         <v>96</v>
@@ -2375,22 +2361,22 @@
         <v>96</v>
       </c>
       <c r="AA2" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AB2" s="55" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AC2" s="55" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AD2" s="18" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="AE2" s="55" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AF2" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AG2" s="12" t="s">
         <v>83</v>
@@ -2695,13 +2681,13 @@
       <c r="EC2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="ED2" s="29" t="s">
+      <c r="ED2" s="30" t="s">
         <v>65</v>
       </c>
       <c r="EE2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="EF2" s="30" t="s">
+      <c r="EF2" s="29" t="s">
         <v>65</v>
       </c>
       <c r="EG2" s="29" t="s">
@@ -2731,14 +2717,8 @@
       <c r="EO2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="EP2" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="EQ2" s="29" t="s">
-        <v>65</v>
-      </c>
     </row>
-    <row r="3" spans="1:147" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:145" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="34" t="s">
         <v>68</v>
       </c>
@@ -2746,7 +2726,7 @@
         <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>106</v>
@@ -2758,7 +2738,7 @@
         <v>102</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>72</v>
@@ -2768,34 +2748,34 @@
         <v>118</v>
       </c>
       <c r="K3" s="43" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="N3" s="65" t="s">
+        <v>384</v>
+      </c>
+      <c r="O3" s="65" t="s">
+        <v>386</v>
+      </c>
+      <c r="P3" s="66" t="s">
         <v>388</v>
       </c>
-      <c r="O3" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="P3" s="66" t="s">
-        <v>392</v>
-      </c>
       <c r="Q3" s="65" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="R3" s="65" t="s">
+        <v>384</v>
+      </c>
+      <c r="S3" s="65" t="s">
+        <v>386</v>
+      </c>
+      <c r="T3" s="66" t="s">
         <v>388</v>
-      </c>
-      <c r="S3" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="T3" s="66" t="s">
-        <v>392</v>
       </c>
       <c r="U3" s="9" t="s">
         <v>20</v>
@@ -2870,10 +2850,10 @@
         <v>36</v>
       </c>
       <c r="AS3" s="49" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AT3" s="49" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AU3" s="54" t="s">
         <v>94</v>
@@ -2894,10 +2874,10 @@
         <v>93</v>
       </c>
       <c r="BA3" s="49" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BB3" s="49" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BC3" s="54" t="s">
         <v>94</v>
@@ -2927,127 +2907,127 @@
         <v>79</v>
       </c>
       <c r="BL3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="BM3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="BM3" s="27" t="s">
+      <c r="BN3" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="BO3" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="BP3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="BQ3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="BR3" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="BS3" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="BT3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="BU3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="BV3" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="BW3" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="BX3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="BY3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="BZ3" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="CA3" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="CB3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="CC3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="CD3" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="CE3" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="CF3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="CG3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="CH3" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="CI3" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="CJ3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="CK3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="CL3" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="CM3" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="CN3" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="CO3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BN3" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="BO3" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="BP3" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="BQ3" s="27" t="s">
+      <c r="CP3" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="CQ3" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="CR3" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="CS3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BR3" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="BS3" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="BT3" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="BU3" s="27" t="s">
+      <c r="CT3" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="CU3" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="CV3" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="CW3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="BV3" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="BW3" s="27" t="s">
-        <v>319</v>
-      </c>
-      <c r="BX3" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="BY3" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="BZ3" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="CA3" s="27" t="s">
-        <v>319</v>
-      </c>
-      <c r="CB3" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="CC3" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="CD3" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="CE3" s="27" t="s">
-        <v>319</v>
-      </c>
-      <c r="CF3" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="CG3" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="CH3" s="27" t="s">
+      <c r="CX3" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="CI3" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="CJ3" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="CK3" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="CL3" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="CM3" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="CN3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="CO3" s="27" t="s">
+      <c r="CY3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="CP3" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="CQ3" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="CR3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="CS3" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="CT3" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="CU3" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="CV3" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="CW3" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="CX3" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="CY3" s="27" t="s">
-        <v>182</v>
-      </c>
       <c r="CZ3" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DA3" s="27" t="s">
         <v>121</v>
@@ -3056,10 +3036,10 @@
         <v>122</v>
       </c>
       <c r="DC3" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="DD3" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DE3" s="27" t="s">
         <v>121</v>
@@ -3068,118 +3048,112 @@
         <v>122</v>
       </c>
       <c r="DG3" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="DH3" s="26" t="s">
         <v>139</v>
       </c>
       <c r="DI3" s="59" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="DJ3" s="26" t="s">
         <v>140</v>
       </c>
       <c r="DK3" s="59" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="DL3" s="26" t="s">
         <v>141</v>
       </c>
       <c r="DM3" s="59" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="DN3" s="26" t="s">
         <v>142</v>
       </c>
       <c r="DO3" s="59" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="DP3" s="26" t="s">
         <v>143</v>
       </c>
       <c r="DQ3" s="59" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="DR3" s="26" t="s">
         <v>144</v>
       </c>
       <c r="DS3" s="59" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="DT3" s="26" t="s">
         <v>145</v>
       </c>
       <c r="DU3" s="59" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="DV3" s="26" t="s">
         <v>146</v>
       </c>
       <c r="DW3" s="59" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="DX3" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="DY3" s="59" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="DZ3" s="26" t="s">
         <v>149</v>
       </c>
       <c r="EA3" s="59" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="EB3" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="EC3" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="ED3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="EC3" s="59" t="s">
-        <v>226</v>
-      </c>
-      <c r="ED3" s="26" t="s">
+      <c r="EE3" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="EF3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="EE3" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="EF3" s="26" t="s">
+      <c r="EG3" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="EH3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="EG3" s="59" t="s">
-        <v>222</v>
-      </c>
-      <c r="EH3" s="26" t="s">
-        <v>154</v>
-      </c>
       <c r="EI3" s="59" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="EJ3" s="26" t="s">
         <v>155</v>
       </c>
       <c r="EK3" s="59" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="EL3" s="26" t="s">
         <v>157</v>
       </c>
       <c r="EM3" s="59" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="EN3" s="26" t="s">
         <v>159</v>
       </c>
       <c r="EO3" s="59" t="s">
-        <v>214</v>
-      </c>
-      <c r="EP3" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="EQ3" s="59" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:147" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:145" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
@@ -3205,7 +3179,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J4" s="38" t="s">
         <v>119</v>
@@ -3217,28 +3191,28 @@
         <v>8</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="N4" s="38" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="O4" s="62" t="s">
         <v>60</v>
       </c>
       <c r="P4" s="44" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Q4" s="38" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="R4" s="38" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="S4" s="38" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="T4" s="44" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="U4" s="38" t="s">
         <v>73</v>
@@ -3259,22 +3233,22 @@
         <v>75</v>
       </c>
       <c r="AA4" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="AB4" s="40" t="s">
+        <v>341</v>
+      </c>
+      <c r="AC4" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="AB4" s="40" t="s">
-        <v>345</v>
-      </c>
-      <c r="AC4" s="40" t="s">
+      <c r="AD4" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="AE4" s="40" t="s">
         <v>346</v>
       </c>
-      <c r="AD4" s="38" t="s">
+      <c r="AF4" s="38" t="s">
         <v>348</v>
-      </c>
-      <c r="AE4" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="AF4" s="38" t="s">
-        <v>352</v>
       </c>
       <c r="AG4" s="38" t="s">
         <v>84</v>
@@ -3295,25 +3269,25 @@
         <v>37</v>
       </c>
       <c r="AM4" s="38" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AN4" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="AO4" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="AP4" s="38" t="s">
         <v>359</v>
       </c>
-      <c r="AO4" s="38" t="s">
+      <c r="AQ4" s="38" t="s">
         <v>361</v>
       </c>
-      <c r="AP4" s="38" t="s">
+      <c r="AR4" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="AQ4" s="38" t="s">
-        <v>365</v>
-      </c>
-      <c r="AR4" s="61" t="s">
-        <v>367</v>
-      </c>
       <c r="AS4" s="38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AT4" s="38" t="s">
         <v>9</v>
@@ -3337,28 +3311,28 @@
         <v>34</v>
       </c>
       <c r="BA4" s="38" t="s">
+        <v>365</v>
+      </c>
+      <c r="BB4" s="38" t="s">
+        <v>367</v>
+      </c>
+      <c r="BC4" s="40" t="s">
         <v>369</v>
       </c>
-      <c r="BB4" s="38" t="s">
-        <v>371</v>
-      </c>
-      <c r="BC4" s="40" t="s">
+      <c r="BD4" s="38" t="s">
+        <v>372</v>
+      </c>
+      <c r="BE4" s="40" t="s">
         <v>373</v>
       </c>
-      <c r="BD4" s="38" t="s">
-        <v>376</v>
-      </c>
-      <c r="BE4" s="40" t="s">
+      <c r="BF4" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="BG4" s="38" t="s">
         <v>377</v>
       </c>
-      <c r="BF4" s="40" t="s">
+      <c r="BH4" s="40" t="s">
         <v>379</v>
-      </c>
-      <c r="BG4" s="38" t="s">
-        <v>381</v>
-      </c>
-      <c r="BH4" s="40" t="s">
-        <v>383</v>
       </c>
       <c r="BI4" s="38" t="s">
         <v>78</v>
@@ -3367,130 +3341,130 @@
         <v>42</v>
       </c>
       <c r="BK4" s="38" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="BL4" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="BM4" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="BN4" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="BO4" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="BP4" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="BQ4" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="BR4" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="BS4" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="BT4" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="BU4" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="BV4" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="BW4" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="BX4" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="BY4" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="BZ4" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="CA4" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="CB4" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="CC4" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="CD4" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="CE4" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="CF4" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="CG4" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="BM4" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="BN4" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="BO4" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="BP4" s="38" t="s">
-        <v>186</v>
-      </c>
-      <c r="BQ4" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="BR4" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="BS4" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="BT4" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="BU4" s="38" t="s">
+      <c r="CH4" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="CI4" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="CJ4" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="CK4" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="CL4" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="CM4" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="CN4" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="BV4" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="BW4" s="38" t="s">
+      <c r="CO4" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="BX4" s="38" t="s">
-        <v>320</v>
-      </c>
-      <c r="BY4" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="BZ4" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="CA4" s="38" t="s">
-        <v>326</v>
-      </c>
-      <c r="CB4" s="38" t="s">
-        <v>328</v>
-      </c>
-      <c r="CC4" s="38" t="s">
-        <v>330</v>
-      </c>
-      <c r="CD4" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="CE4" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="CF4" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="CG4" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="CH4" s="38" t="s">
+      <c r="CP4" s="38" t="s">
         <v>287</v>
       </c>
-      <c r="CI4" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="CJ4" s="38" t="s">
-        <v>300</v>
-      </c>
-      <c r="CK4" s="38" t="s">
-        <v>303</v>
-      </c>
-      <c r="CL4" s="38" t="s">
-        <v>305</v>
-      </c>
-      <c r="CM4" s="38" t="s">
+      <c r="CQ4" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="CR4" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="CS4" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="CT4" s="38" t="s">
+        <v>288</v>
+      </c>
+      <c r="CU4" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="CV4" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="CN4" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="CO4" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="CP4" s="38" t="s">
-        <v>291</v>
-      </c>
-      <c r="CQ4" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="CR4" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="CS4" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="CT4" s="38" t="s">
-        <v>292</v>
-      </c>
-      <c r="CU4" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="CV4" s="38" t="s">
+      <c r="CW4" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="CX4" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="CW4" s="38" t="s">
+      <c r="CY4" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="CX4" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="CY4" s="38" t="s">
-        <v>317</v>
-      </c>
       <c r="CZ4" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="DA4" s="38" t="s">
         <v>123</v>
@@ -3499,10 +3473,10 @@
         <v>124</v>
       </c>
       <c r="DC4" s="38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="DD4" s="38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="DE4" s="38" t="s">
         <v>125</v>
@@ -3511,118 +3485,112 @@
         <v>126</v>
       </c>
       <c r="DG4" s="38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="DH4" s="38" t="s">
         <v>52</v>
       </c>
       <c r="DI4" s="38" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="DJ4" s="38" t="s">
         <v>56</v>
       </c>
       <c r="DK4" s="38" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="DL4" s="41" t="s">
         <v>59</v>
       </c>
       <c r="DM4" s="38" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="DN4" s="38" t="s">
         <v>54</v>
       </c>
       <c r="DO4" s="38" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="DP4" s="38" t="s">
         <v>55</v>
       </c>
       <c r="DQ4" s="38" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="DR4" s="41" t="s">
         <v>58</v>
       </c>
       <c r="DS4" s="38" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="DT4" s="41" t="s">
         <v>114</v>
       </c>
       <c r="DU4" s="38" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="DV4" s="41" t="s">
         <v>62</v>
       </c>
       <c r="DW4" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="DX4" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="DY4" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="DZ4" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="EA4" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="EB4" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="EC4" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="DX4" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="DY4" s="38" t="s">
+      <c r="ED4" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="EE4" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="DZ4" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="EA4" s="38" t="s">
+      <c r="EF4" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="EG4" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="EB4" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="EC4" s="38" t="s">
+      <c r="EH4" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="EI4" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="ED4" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="EE4" s="38" t="s">
+      <c r="EJ4" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="EK4" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="EF4" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="EG4" s="38" t="s">
+      <c r="EL4" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="EM4" s="41" t="s">
         <v>260</v>
       </c>
-      <c r="EH4" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="EI4" s="38" t="s">
+      <c r="EN4" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="EO4" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="EJ4" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="EK4" s="38" t="s">
-        <v>262</v>
-      </c>
-      <c r="EL4" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="EM4" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="EN4" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="EO4" s="41" t="s">
-        <v>264</v>
-      </c>
-      <c r="EP4" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="EQ4" s="38" t="s">
-        <v>265</v>
-      </c>
     </row>
-    <row r="5" spans="1:147" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:145" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="35" t="s">
         <v>67</v>
       </c>
@@ -3648,76 +3616,76 @@
         <v>15</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="58" t="s">
+        <v>381</v>
+      </c>
+      <c r="N5" s="58" t="s">
         <v>385</v>
       </c>
-      <c r="N5" s="58" t="s">
-        <v>389</v>
-      </c>
       <c r="O5" s="58" t="s">
+        <v>393</v>
+      </c>
+      <c r="P5" s="46" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q5" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="R5" s="58" t="s">
+        <v>395</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="T5" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="P5" s="46" t="s">
-        <v>392</v>
-      </c>
-      <c r="Q5" s="58" t="s">
-        <v>398</v>
-      </c>
-      <c r="R5" s="58" t="s">
-        <v>399</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="T5" s="46" t="s">
-        <v>401</v>
-      </c>
       <c r="U5" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="V5" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="W5" s="53" t="s">
+        <v>334</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y5" s="53" t="s">
         <v>336</v>
       </c>
-      <c r="V5" s="53" t="s">
+      <c r="Z5" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="W5" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="X5" s="6" t="s">
+      <c r="AA5" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="Y5" s="53" t="s">
+      <c r="AB5" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="Z5" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AC5" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="AB5" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="AC5" s="53" t="s">
+      <c r="AD5" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE5" s="53" t="s">
         <v>347</v>
       </c>
-      <c r="AD5" s="6" t="s">
+      <c r="AF5" s="4" t="s">
         <v>349</v>
-      </c>
-      <c r="AE5" s="53" t="s">
-        <v>351</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>353</v>
       </c>
       <c r="AG5" s="4" t="s">
         <v>110</v>
@@ -3738,25 +3706,25 @@
         <v>4</v>
       </c>
       <c r="AM5" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="AN5" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="AO5" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="AP5" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="AO5" s="6" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AR5" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="AQ5" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>368</v>
-      </c>
       <c r="AS5" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AT5" s="4" t="s">
         <v>29</v>
@@ -3780,28 +3748,28 @@
         <v>91</v>
       </c>
       <c r="BA5" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="BC5" s="53" t="s">
         <v>370</v>
       </c>
-      <c r="BB5" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="BC5" s="53" t="s">
+      <c r="BD5" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="BE5" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="BD5" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="BE5" s="53" t="s">
+      <c r="BF5" s="53" t="s">
+        <v>376</v>
+      </c>
+      <c r="BG5" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="BF5" s="53" t="s">
+      <c r="BH5" s="53" t="s">
         <v>380</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="BH5" s="53" t="s">
-        <v>384</v>
       </c>
       <c r="BI5" s="4" t="s">
         <v>113</v>
@@ -3813,127 +3781,127 @@
         <v>44</v>
       </c>
       <c r="BL5" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="BM5" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="BN5" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="BO5" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="BP5" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="BQ5" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BR5" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="BS5" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="BT5" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="BM5" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="BN5" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="BO5" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="BP5" s="4" t="s">
+      <c r="BU5" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="BQ5" s="4" t="s">
+      <c r="BV5" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="BW5" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="BR5" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="BS5" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="BT5" s="4" t="s">
+      <c r="BX5" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="BY5" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="BZ5" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="CA5" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="CB5" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="CC5" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="CD5" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="CE5" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="CF5" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="CG5" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="CH5" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="CI5" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="CJ5" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="CK5" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="CL5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="CM5" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="CN5" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="CO5" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="CP5" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="CQ5" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="CR5" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="CS5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="CT5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="CU5" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="BU5" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="BV5" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="BW5" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="BX5" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="BY5" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="BZ5" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="CA5" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="CB5" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="CC5" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="CD5" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="CE5" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="CF5" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="CG5" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="CH5" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="CI5" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="CJ5" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="CK5" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="CL5" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="CM5" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="CN5" s="4" t="s">
+      <c r="CV5" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="CO5" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="CP5" s="4" t="s">
+      <c r="CW5" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="CQ5" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="CR5" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="CS5" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="CT5" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="CU5" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="CV5" s="4" t="s">
+      <c r="CX5" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="CW5" s="4" t="s">
+      <c r="CY5" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="CX5" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="CY5" s="4" t="s">
-        <v>318</v>
-      </c>
       <c r="CZ5" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="DA5" s="4" t="s">
         <v>127</v>
@@ -3942,10 +3910,10 @@
         <v>128</v>
       </c>
       <c r="DC5" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="DD5" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="DE5" s="4" t="s">
         <v>129</v>
@@ -3954,119 +3922,113 @@
         <v>130</v>
       </c>
       <c r="DG5" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="DH5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="DI5" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="DJ5" s="4" t="s">
         <v>46</v>
       </c>
       <c r="DK5" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="DL5" s="7" t="s">
         <v>49</v>
       </c>
       <c r="DM5" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DN5" s="4" t="s">
         <v>80</v>
       </c>
       <c r="DO5" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="DP5" s="4" t="s">
         <v>45</v>
       </c>
       <c r="DQ5" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="DR5" s="7" t="s">
         <v>48</v>
       </c>
       <c r="DS5" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="DT5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="DU5" s="4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="DV5" s="7" t="s">
         <v>81</v>
       </c>
       <c r="DW5" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="DX5" s="7" t="s">
-        <v>147</v>
+        <v>229</v>
+      </c>
+      <c r="DX5" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="DY5" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="DZ5" s="4" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="EA5" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="EB5" s="4" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="EC5" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="ED5" s="4" t="s">
-        <v>117</v>
+        <v>223</v>
+      </c>
+      <c r="ED5" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="EE5" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="EF5" s="14" t="s">
-        <v>89</v>
+        <v>221</v>
+      </c>
+      <c r="EF5" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="EG5" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="EH5" s="4" t="s">
-        <v>66</v>
+        <v>218</v>
+      </c>
+      <c r="EH5" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="EI5" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="EJ5" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="EJ5" s="4" t="s">
         <v>156</v>
       </c>
       <c r="EK5" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="EL5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="EL5" s="7" t="s">
         <v>158</v>
       </c>
       <c r="EM5" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="EN5" s="7" t="s">
         <v>160</v>
       </c>
       <c r="EO5" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="EP5" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="EQ5" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:147" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="7" spans="1:147" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:145" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:145" x14ac:dyDescent="0.55000000000000004">
       <c r="G7" s="32"/>
     </row>
   </sheetData>
@@ -4084,7 +4046,7 @@
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 EO6:EO1048576 EM6:EM1048576 EQ6:EQ1048576 EK6:EK1048576 EI6:EI1048576 EG6:EG1048576 EE6:EE1048576 EC6:EC1048576 EA6:EA1048576 DY6:DY1048576 DW6:DW1048576 DU6:DU1048576 DS6:DS1048576 DQ6:DQ1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 DI6:DI1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 EM6:EM1048576 EK6:EK1048576 EO6:EO1048576 EI6:EI1048576 EG6:EG1048576 EE6:EE1048576 EC6:EC1048576 EA6:EA1048576 DY6:DY1048576 DW6:DW1048576 DU6:DU1048576 DS6:DS1048576 DQ6:DQ1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 DI6:DI1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4180,17 +4142,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>